<commit_message>
update project structure and add excel parsing and inserting in db
</commit_message>
<xml_diff>
--- a/data/downloads/Adani Ports.xlsx
+++ b/data/downloads/Adani Ports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratyush/Websites/screener/company/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\finance_project\data\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AC4F62-F3F6-2E4B-8F69-3E72AC5D7A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84EAF486-6F84-4425-8E5E-118381173088}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profit &amp; Loss" sheetId="1" r:id="rId1"/>
@@ -28,13 +28,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -342,8 +335,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
@@ -464,7 +457,7 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -476,19 +469,19 @@
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -498,13 +491,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -518,11 +511,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,7 +526,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="6" builtinId="5"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
@@ -1724,26 +1717,28 @@
       <selection activeCell="I2" sqref="I2"/>
       <selection pane="topRight" activeCell="I2" sqref="I2"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
-      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="6" customWidth="1"/>
-    <col min="2" max="6" width="13.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.5" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" style="6" customWidth="1"/>
-    <col min="13" max="14" width="12.1640625" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="20.7109375" style="6" customWidth="1"/>
+    <col min="2" max="6" width="13.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.42578125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="6" customWidth="1"/>
+    <col min="13" max="14" width="12.140625" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="str">
         <f>'Data Sheet'!B1</f>
+        <v>ADANI PORTS &amp; SPECIAL ECONOMIC ZONE LTD</v>
       </c>
       <c r="H1" t="str">
         <f>UPDATE</f>
+        <v/>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -1751,39 +1746,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16">
         <f>'Data Sheet'!B16</f>
+        <v>42460</v>
       </c>
       <c r="C3" s="16">
         <f>'Data Sheet'!C16</f>
+        <v>42825</v>
       </c>
       <c r="D3" s="16">
         <f>'Data Sheet'!D16</f>
+        <v>43190</v>
       </c>
       <c r="E3" s="16">
         <f>'Data Sheet'!E16</f>
+        <v>43555</v>
       </c>
       <c r="F3" s="16">
         <f>'Data Sheet'!F16</f>
+        <v>43921</v>
       </c>
       <c r="G3" s="16">
         <f>'Data Sheet'!G16</f>
+        <v>44286</v>
       </c>
       <c r="H3" s="16">
         <f>'Data Sheet'!H16</f>
+        <v>44651</v>
       </c>
       <c r="I3" s="16">
         <f>'Data Sheet'!I16</f>
+        <v>45016</v>
       </c>
       <c r="J3" s="16">
         <f>'Data Sheet'!J16</f>
+        <v>45382</v>
       </c>
       <c r="K3" s="16">
         <f>'Data Sheet'!K16</f>
+        <v>45747</v>
       </c>
       <c r="L3" s="17" t="s">
         <v>3</v>
@@ -1795,174 +1800,224 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
         <f>'Data Sheet'!B17</f>
+        <v>7108.65</v>
       </c>
       <c r="C4" s="1">
         <f>'Data Sheet'!C17</f>
+        <v>8439.35</v>
       </c>
       <c r="D4" s="1">
         <f>'Data Sheet'!D17</f>
+        <v>11322.96</v>
       </c>
       <c r="E4" s="1">
         <f>'Data Sheet'!E17</f>
+        <v>10925.44</v>
       </c>
       <c r="F4" s="1">
         <f>'Data Sheet'!F17</f>
+        <v>11873.07</v>
       </c>
       <c r="G4" s="1">
         <f>'Data Sheet'!G17</f>
+        <v>12549.6</v>
       </c>
       <c r="H4" s="1">
         <f>'Data Sheet'!H17</f>
+        <v>17118.79</v>
       </c>
       <c r="I4" s="1">
         <f>'Data Sheet'!I17</f>
+        <v>20851.91</v>
       </c>
       <c r="J4" s="1">
         <f>'Data Sheet'!J17</f>
+        <v>26710.560000000001</v>
       </c>
       <c r="K4" s="1">
         <f>'Data Sheet'!K17</f>
+        <v>30475.33</v>
       </c>
       <c r="L4" s="1">
         <f>SUM(Quarters!H4:K4)</f>
+        <v>31078.6</v>
       </c>
       <c r="M4" s="1">
         <f>$K4+M23*K4</f>
+        <v>36935.178419121592</v>
       </c>
       <c r="N4" s="1">
         <f>$K4+N23*L4</f>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>34855.761594170996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="9">
         <f>SUM('Data Sheet'!B18,'Data Sheet'!B20:B24, -1*'Data Sheet'!B19)</f>
+        <v>2531.7000000000003</v>
       </c>
       <c r="C5" s="9">
         <f>SUM('Data Sheet'!C18,'Data Sheet'!C20:C24, -1*'Data Sheet'!C19)</f>
+        <v>3021.12</v>
       </c>
       <c r="D5" s="9">
         <f>SUM('Data Sheet'!D18,'Data Sheet'!D20:D24, -1*'Data Sheet'!D19)</f>
+        <v>4166.29</v>
       </c>
       <c r="E5" s="9">
         <f>SUM('Data Sheet'!E18,'Data Sheet'!E20:E24, -1*'Data Sheet'!E19)</f>
+        <v>4329.8</v>
       </c>
       <c r="F5" s="9">
         <f>SUM('Data Sheet'!F18,'Data Sheet'!F20:F24, -1*'Data Sheet'!F19)</f>
+        <v>5925.96</v>
       </c>
       <c r="G5" s="9">
         <f>SUM('Data Sheet'!G18,'Data Sheet'!G20:G24, -1*'Data Sheet'!G19)</f>
+        <v>3861.6399999999994</v>
       </c>
       <c r="H5" s="9">
         <f>SUM('Data Sheet'!H18,'Data Sheet'!H20:H24, -1*'Data Sheet'!H19)</f>
+        <v>7590.83</v>
       </c>
       <c r="I5" s="9">
         <f>SUM('Data Sheet'!I18,'Data Sheet'!I20:I24, -1*'Data Sheet'!I19)</f>
+        <v>9904.7800000000007</v>
       </c>
       <c r="J5" s="9">
         <f>SUM('Data Sheet'!J18,'Data Sheet'!J20:J24, -1*'Data Sheet'!J19)</f>
+        <v>11121.149999999998</v>
       </c>
       <c r="K5" s="9">
         <f>SUM('Data Sheet'!K18,'Data Sheet'!K20:K24, -1*'Data Sheet'!K19)</f>
+        <v>12334.810000000001</v>
       </c>
       <c r="L5" s="9">
         <f>SUM(Quarters!H5:K5)</f>
+        <v>12295.89</v>
       </c>
       <c r="M5" s="9">
         <f t="shared" ref="M5:N5" si="0">M4-M6</f>
+        <v>14612.977771582147</v>
       </c>
       <c r="N5" s="9">
         <f t="shared" si="0"/>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>14900.650710875037</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
         <f>B4-B5</f>
+        <v>4576.9499999999989</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ref="C6:K6" si="1">C4-C5</f>
+        <v>5418.2300000000005</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
+        <v>7156.6699999999992</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
+        <v>6595.64</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
+        <v>5947.11</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
+        <v>8687.9600000000009</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
+        <v>9527.9600000000009</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
+        <v>10947.13</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
+        <v>15589.410000000003</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="1"/>
+        <v>18140.52</v>
       </c>
       <c r="L6" s="1">
         <f>SUM(Quarters!H6:K6)</f>
+        <v>18782.71</v>
       </c>
       <c r="M6" s="1">
         <f>M4*M24</f>
+        <v>22322.200647539445</v>
       </c>
       <c r="N6" s="1">
         <f>N4*N24</f>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>19955.110883295958</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="9">
         <f>'Data Sheet'!B25</f>
+        <v>729.75</v>
       </c>
       <c r="C7" s="9">
         <f>'Data Sheet'!C25</f>
+        <v>1036.57</v>
       </c>
       <c r="D7" s="9">
         <f>'Data Sheet'!D25</f>
+        <v>844.49</v>
       </c>
       <c r="E7" s="9">
         <f>'Data Sheet'!E25</f>
+        <v>1289.25</v>
       </c>
       <c r="F7" s="9">
         <f>'Data Sheet'!F25</f>
+        <v>1927.73</v>
       </c>
       <c r="G7" s="9">
         <f>'Data Sheet'!G25</f>
+        <v>1966.68</v>
       </c>
       <c r="H7" s="9">
         <f>'Data Sheet'!H25</f>
+        <v>1832.4</v>
       </c>
       <c r="I7" s="9">
         <f>'Data Sheet'!I25</f>
+        <v>327.11</v>
       </c>
       <c r="J7" s="9">
         <f>'Data Sheet'!J25</f>
+        <v>670.56</v>
       </c>
       <c r="K7" s="9">
         <f>'Data Sheet'!K25</f>
+        <v>1799.85</v>
       </c>
       <c r="L7" s="9">
         <f>SUM(Quarters!H7:K7)</f>
+        <v>1275.21</v>
       </c>
       <c r="M7" s="9">
         <v>0</v>
@@ -1971,437 +2026,562 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="9">
         <f>'Data Sheet'!B26</f>
+        <v>1062.96</v>
       </c>
       <c r="C8" s="9">
         <f>'Data Sheet'!C26</f>
+        <v>1160.19</v>
       </c>
       <c r="D8" s="9">
         <f>'Data Sheet'!D26</f>
+        <v>1188.3699999999999</v>
       </c>
       <c r="E8" s="9">
         <f>'Data Sheet'!E26</f>
+        <v>1373.48</v>
       </c>
       <c r="F8" s="9">
         <f>'Data Sheet'!F26</f>
+        <v>1680.28</v>
       </c>
       <c r="G8" s="9">
         <f>'Data Sheet'!G26</f>
+        <v>2107.34</v>
       </c>
       <c r="H8" s="9">
         <f>'Data Sheet'!H26</f>
+        <v>3099.3</v>
       </c>
       <c r="I8" s="9">
         <f>'Data Sheet'!I26</f>
+        <v>3424.71</v>
       </c>
       <c r="J8" s="9">
         <f>'Data Sheet'!J26</f>
+        <v>3888.46</v>
       </c>
       <c r="K8" s="9">
         <f>'Data Sheet'!K26</f>
+        <v>4378.93</v>
       </c>
       <c r="L8" s="9">
         <f>SUM(Quarters!H8:K8)</f>
+        <v>4378.93</v>
       </c>
       <c r="M8" s="9">
         <f>+$L8</f>
+        <v>4378.93</v>
       </c>
       <c r="N8" s="9">
         <f>+$L8</f>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4378.93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9">
         <f>'Data Sheet'!B27</f>
+        <v>1124.3</v>
       </c>
       <c r="C9" s="9">
         <f>'Data Sheet'!C27</f>
+        <v>1115.74</v>
       </c>
       <c r="D9" s="9">
         <f>'Data Sheet'!D27</f>
+        <v>1578.66</v>
       </c>
       <c r="E9" s="9">
         <f>'Data Sheet'!E27</f>
+        <v>1385.19</v>
       </c>
       <c r="F9" s="9">
         <f>'Data Sheet'!F27</f>
+        <v>1950.64</v>
       </c>
       <c r="G9" s="9">
         <f>'Data Sheet'!G27</f>
+        <v>2255.29</v>
       </c>
       <c r="H9" s="9">
         <f>'Data Sheet'!H27</f>
+        <v>2543.92</v>
       </c>
       <c r="I9" s="9">
         <f>'Data Sheet'!I27</f>
+        <v>2362.64</v>
       </c>
       <c r="J9" s="9">
         <f>'Data Sheet'!J27</f>
+        <v>2732.94</v>
       </c>
       <c r="K9" s="9">
         <f>'Data Sheet'!K27</f>
+        <v>2531.8200000000002</v>
       </c>
       <c r="L9" s="9">
         <f>SUM(Quarters!H9:K9)</f>
+        <v>2649.37</v>
       </c>
       <c r="M9" s="9">
         <f>+$L9</f>
+        <v>2649.37</v>
       </c>
       <c r="N9" s="9">
         <f>+$L9</f>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2649.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="9">
         <f>'Data Sheet'!B28</f>
+        <v>3119.44</v>
       </c>
       <c r="C10" s="9">
         <f>'Data Sheet'!C28</f>
+        <v>4178.87</v>
       </c>
       <c r="D10" s="9">
         <f>'Data Sheet'!D28</f>
+        <v>5234.13</v>
       </c>
       <c r="E10" s="9">
         <f>'Data Sheet'!E28</f>
+        <v>5126.22</v>
       </c>
       <c r="F10" s="9">
         <f>'Data Sheet'!F28</f>
+        <v>4243.92</v>
       </c>
       <c r="G10" s="9">
         <f>'Data Sheet'!G28</f>
+        <v>6292.01</v>
       </c>
       <c r="H10" s="9">
         <f>'Data Sheet'!H28</f>
+        <v>5717.14</v>
       </c>
       <c r="I10" s="9">
         <f>'Data Sheet'!I28</f>
+        <v>5486.89</v>
       </c>
       <c r="J10" s="9">
         <f>'Data Sheet'!J28</f>
+        <v>9638.57</v>
       </c>
       <c r="K10" s="9">
         <f>'Data Sheet'!K28</f>
+        <v>13029.62</v>
       </c>
       <c r="L10" s="9">
         <f>SUM(Quarters!H10:K10)</f>
+        <v>13029.619999999999</v>
       </c>
       <c r="M10" s="9">
         <f>M6+M7-SUM(M8:M9)</f>
+        <v>15293.900647539445</v>
       </c>
       <c r="N10" s="9">
         <f>N6+N7-SUM(N8:N9)</f>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>12926.810883295959</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="9">
         <f>'Data Sheet'!B29</f>
+        <v>282.81</v>
       </c>
       <c r="C11" s="9">
         <f>'Data Sheet'!C29</f>
+        <v>286.63</v>
       </c>
       <c r="D11" s="9">
         <f>'Data Sheet'!D29</f>
+        <v>1544.18</v>
       </c>
       <c r="E11" s="9">
         <f>'Data Sheet'!E29</f>
+        <v>1081.47</v>
       </c>
       <c r="F11" s="9">
         <f>'Data Sheet'!F29</f>
+        <v>459.39</v>
       </c>
       <c r="G11" s="9">
         <f>'Data Sheet'!G29</f>
+        <v>1243.27</v>
       </c>
       <c r="H11" s="9">
         <f>'Data Sheet'!H29</f>
+        <v>763.96</v>
       </c>
       <c r="I11" s="9">
         <f>'Data Sheet'!I29</f>
+        <v>96.04</v>
       </c>
       <c r="J11" s="9">
         <f>'Data Sheet'!J29</f>
+        <v>1534.58</v>
       </c>
       <c r="K11" s="9">
         <f>'Data Sheet'!K29</f>
+        <v>1968.36</v>
       </c>
       <c r="L11" s="9">
         <f>SUM(Quarters!H11:K11)</f>
+        <v>1968.36</v>
       </c>
       <c r="M11" s="10">
         <f>IF($L10&gt;0,$L11/$L10,0)</f>
+        <v>0.1510681048257739</v>
       </c>
       <c r="N11" s="10">
         <f>IF($L10&gt;0,$L11/$L10,0)</f>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.1510681048257739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1">
         <f>'Data Sheet'!B30</f>
+        <v>2897.16</v>
       </c>
       <c r="C12" s="1">
         <f>'Data Sheet'!C30</f>
+        <v>3911.52</v>
       </c>
       <c r="D12" s="1">
         <f>'Data Sheet'!D30</f>
+        <v>3673.62</v>
       </c>
       <c r="E12" s="1">
         <f>'Data Sheet'!E30</f>
+        <v>3990.22</v>
       </c>
       <c r="F12" s="1">
         <f>'Data Sheet'!F30</f>
+        <v>3763.13</v>
       </c>
       <c r="G12" s="1">
         <f>'Data Sheet'!G30</f>
+        <v>4994.3</v>
       </c>
       <c r="H12" s="1">
         <f>'Data Sheet'!H30</f>
+        <v>4886.03</v>
       </c>
       <c r="I12" s="1">
         <f>'Data Sheet'!I30</f>
+        <v>5308.85</v>
       </c>
       <c r="J12" s="1">
         <f>'Data Sheet'!J30</f>
+        <v>8110.64</v>
       </c>
       <c r="K12" s="1">
         <f>'Data Sheet'!K30</f>
+        <v>11092.31</v>
       </c>
       <c r="L12" s="1">
         <f>SUM(Quarters!H12:K12)</f>
+        <v>11092.31</v>
       </c>
       <c r="M12" s="1">
         <f>M10-M11*M10</f>
+        <v>12983.480061321985</v>
       </c>
       <c r="N12" s="1">
         <f>N10-N11*N10</f>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10973.982061715251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="9">
         <f>IF('Data Sheet'!B93&gt;0,B12/'Data Sheet'!B93,0)</f>
+        <v>13.989183969097054</v>
       </c>
       <c r="C13" s="9">
         <f>IF('Data Sheet'!C93&gt;0,C12/'Data Sheet'!C93,0)</f>
+        <v>18.887107677450508</v>
       </c>
       <c r="D13" s="9">
         <f>IF('Data Sheet'!D93&gt;0,D12/'Data Sheet'!D93,0)</f>
+        <v>17.738387252535006</v>
       </c>
       <c r="E13" s="9">
         <f>IF('Data Sheet'!E93&gt;0,E12/'Data Sheet'!E93,0)</f>
+        <v>19.267117334620956</v>
       </c>
       <c r="F13" s="9">
         <f>IF('Data Sheet'!F93&gt;0,F12/'Data Sheet'!F93,0)</f>
+        <v>18.521163500344521</v>
       </c>
       <c r="G13" s="9">
         <f>IF('Data Sheet'!G93&gt;0,G12/'Data Sheet'!G93,0)</f>
+        <v>24.580667388522492</v>
       </c>
       <c r="H13" s="9">
         <f>IF('Data Sheet'!H93&gt;0,H12/'Data Sheet'!H93,0)</f>
+        <v>23.130231016852868</v>
       </c>
       <c r="I13" s="9">
         <f>IF('Data Sheet'!I93&gt;0,I12/'Data Sheet'!I93,0)</f>
+        <v>24.576871441136987</v>
       </c>
       <c r="J13" s="9">
         <f>IF('Data Sheet'!J93&gt;0,J12/'Data Sheet'!J93,0)</f>
+        <v>37.547520948104257</v>
       </c>
       <c r="K13" s="9">
         <f>IF('Data Sheet'!K93&gt;0,K12/'Data Sheet'!K93,0)</f>
+        <v>51.350909680107399</v>
       </c>
       <c r="L13" s="9">
         <f>IF('Data Sheet'!$B6&gt;0,'Profit &amp; Loss'!L12/'Data Sheet'!$B6,0)</f>
+        <v>51.349977761004858</v>
       </c>
       <c r="M13" s="9">
         <f>IF('Data Sheet'!$B6&gt;0,'Profit &amp; Loss'!M12/'Data Sheet'!$B6,0)</f>
+        <v>60.104830500530007</v>
       </c>
       <c r="N13" s="9">
         <f>IF('Data Sheet'!$B6&gt;0,'Profit &amp; Loss'!N12/'Data Sheet'!$B6,0)</f>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>50.802198533826086</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9" t="str">
+      <c r="B14" s="9">
         <f>IF(B15&gt;0,B15/B13,"")</f>
-      </c>
-      <c r="C14" s="9" t="str">
+        <v>17.70653674633089</v>
+      </c>
+      <c r="C14" s="9">
         <f t="shared" ref="C14:K14" si="2">IF(C15&gt;0,C15/C13,"")</f>
-      </c>
-      <c r="D14" s="9" t="str">
+        <v>17.980519082095963</v>
+      </c>
+      <c r="D14" s="9">
         <f t="shared" si="2"/>
-      </c>
-      <c r="E14" s="9" t="str">
+        <v>19.962355932295669</v>
+      </c>
+      <c r="E14" s="9">
         <f t="shared" si="2"/>
-      </c>
-      <c r="F14" s="9" t="str">
+        <v>19.626703540155681</v>
+      </c>
+      <c r="F14" s="9">
         <f t="shared" si="2"/>
-      </c>
-      <c r="G14" s="9" t="str">
+        <v>13.568262058446029</v>
+      </c>
+      <c r="G14" s="9">
         <f t="shared" si="2"/>
-      </c>
-      <c r="H14" s="9" t="str">
+        <v>28.575302244558795</v>
+      </c>
+      <c r="H14" s="9">
         <f t="shared" si="2"/>
-      </c>
-      <c r="I14" s="9" t="str">
+        <v>33.47134749479639</v>
+      </c>
+      <c r="I14" s="9">
         <f t="shared" si="2"/>
-      </c>
-      <c r="J14" s="9" t="str">
+        <v>25.711165129924556</v>
+      </c>
+      <c r="J14" s="9">
         <f t="shared" si="2"/>
-      </c>
-      <c r="K14" s="9" t="str">
+        <v>35.737379356006429</v>
+      </c>
+      <c r="K14" s="9">
         <f t="shared" si="2"/>
+        <v>23.036592873801762</v>
       </c>
       <c r="L14" s="9">
         <f t="shared" ref="L14" si="3">IF(L13&gt;0,L15/L13,0)</f>
+        <v>26.147041508937278</v>
       </c>
       <c r="M14" s="9">
         <f>M25</f>
+        <v>27.658044717167506</v>
       </c>
       <c r="N14" s="9">
         <f>N25</f>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>23.774836906122676</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="1">
         <f>'Data Sheet'!B90</f>
+        <v>247.7</v>
       </c>
       <c r="C15" s="1">
         <f>'Data Sheet'!C90</f>
+        <v>339.6</v>
       </c>
       <c r="D15" s="1">
         <f>'Data Sheet'!D90</f>
+        <v>354.1</v>
       </c>
       <c r="E15" s="1">
         <f>'Data Sheet'!E90</f>
+        <v>378.15</v>
       </c>
       <c r="F15" s="1">
         <f>'Data Sheet'!F90</f>
+        <v>251.3</v>
       </c>
       <c r="G15" s="1">
         <f>'Data Sheet'!G90</f>
+        <v>702.4</v>
       </c>
       <c r="H15" s="1">
         <f>'Data Sheet'!H90</f>
+        <v>774.2</v>
       </c>
       <c r="I15" s="1">
         <f>'Data Sheet'!I90</f>
+        <v>631.9</v>
       </c>
       <c r="J15" s="1">
         <f>'Data Sheet'!J90</f>
+        <v>1341.85</v>
       </c>
       <c r="K15" s="1">
         <f>'Data Sheet'!K90</f>
+        <v>1182.95</v>
       </c>
       <c r="L15" s="1">
         <f>'Data Sheet'!B8</f>
+        <v>1342.65</v>
       </c>
       <c r="M15" s="12">
         <f>M13*M14</f>
+        <v>1662.3820897014323</v>
       </c>
       <c r="N15" s="13">
         <f>N13*N14</f>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1207.8139846141798</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="7">
         <f>IF('Data Sheet'!B30&gt;0, 'Data Sheet'!B31/'Data Sheet'!B30, 0)</f>
+        <v>7.8628726062764928E-2</v>
       </c>
       <c r="C18" s="7">
         <f>IF('Data Sheet'!C30&gt;0, 'Data Sheet'!C31/'Data Sheet'!C30, 0)</f>
+        <v>6.882746349245307E-2</v>
       </c>
       <c r="D18" s="7">
         <f>IF('Data Sheet'!D30&gt;0, 'Data Sheet'!D31/'Data Sheet'!D30, 0)</f>
+        <v>0.11274709959113899</v>
       </c>
       <c r="E18" s="7">
         <f>IF('Data Sheet'!E30&gt;0, 'Data Sheet'!E31/'Data Sheet'!E30, 0)</f>
+        <v>1.0380380029171325E-2</v>
       </c>
       <c r="F18" s="7">
         <f>IF('Data Sheet'!F30&gt;0, 'Data Sheet'!F31/'Data Sheet'!F30, 0)</f>
+        <v>0.17277107089045554</v>
       </c>
       <c r="G18" s="7">
         <f>IF('Data Sheet'!G30&gt;0, 'Data Sheet'!G31/'Data Sheet'!G30, 0)</f>
+        <v>0.20340788498888732</v>
       </c>
       <c r="H18" s="7">
         <f>IF('Data Sheet'!H30&gt;0, 'Data Sheet'!H31/'Data Sheet'!H30, 0)</f>
+        <v>0.21616322454016862</v>
       </c>
       <c r="I18" s="7">
         <f>IF('Data Sheet'!I30&gt;0, 'Data Sheet'!I31/'Data Sheet'!I30, 0)</f>
+        <v>0.20344895787223219</v>
       </c>
       <c r="J18" s="7">
         <f>IF('Data Sheet'!J30&gt;0, 'Data Sheet'!J31/'Data Sheet'!J30, 0)</f>
+        <v>0.15980119941213022</v>
       </c>
       <c r="K18" s="7">
         <f>IF('Data Sheet'!K30&gt;0, 'Data Sheet'!K31/'Data Sheet'!K30, 0)</f>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.13631966650769767</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="7">
         <f t="shared" ref="B19:L19" si="4">IF(B6&gt;0,B6/B4,0)</f>
+        <v>0.64385642843577884</v>
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:K19" si="5">IF(C6&gt;0,C6/C4,0)</f>
+        <v>0.64201982380159617</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="5"/>
+        <v>0.63204939344482358</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="5"/>
+        <v>0.60369559486849045</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="5"/>
+        <v>0.50089067107327756</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="5"/>
+        <v>0.69228979409702307</v>
       </c>
       <c r="H19" s="7">
         <f t="shared" si="5"/>
+        <v>0.55657905728150181</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" si="5"/>
+        <v>0.52499411324909806</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="5"/>
+        <v>0.58364219993890065</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="5"/>
+        <v>0.59525261908566696</v>
       </c>
       <c r="L19" s="7">
         <f t="shared" si="4"/>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.60436152207628402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -2414,7 +2594,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -2427,7 +2607,7 @@
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
     </row>
-    <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -2459,7 +2639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -2469,78 +2649,99 @@
       <c r="G23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="7" t="str">
+      <c r="H23" s="7">
         <f>IF(B4=0,"",POWER($K4/B4,1/9)-1)</f>
-      </c>
-      <c r="I23" s="7" t="str">
+        <v>0.17554739326307089</v>
+      </c>
+      <c r="I23" s="7">
         <f>IF(D4=0,"",POWER($K4/D4,1/7)-1)</f>
-      </c>
-      <c r="J23" s="7" t="str">
+        <v>0.15193220601280966</v>
+      </c>
+      <c r="J23" s="7">
         <f>IF(F4=0,"",POWER($K4/F4,1/5)-1)</f>
-      </c>
-      <c r="K23" s="7" t="str">
+        <v>0.20747202514220509</v>
+      </c>
+      <c r="K23" s="7">
         <f>IF(H4=0,"",POWER($K4/H4, 1/3)-1)</f>
-      </c>
-      <c r="L23" s="7" t="str">
+        <v>0.2119697610861504</v>
+      </c>
+      <c r="L23" s="7">
         <f>IF(ISERROR(MAX(IF(J4=0,"",(K4-J4)/J4),IF(K4=0,"",(L4-K4)/K4))),"",MAX(IF(J4=0,"",(K4-J4)/J4),IF(K4=0,"",(L4-K4)/K4)))</f>
+        <v>0.14094687644137749</v>
       </c>
       <c r="M23" s="22">
         <f>MAX(K23:L23)</f>
+        <v>0.2119697610861504</v>
       </c>
       <c r="N23" s="22">
         <f>MIN(H23:L23)</f>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.14094687644137749</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="7" t="str">
+      <c r="H24" s="7">
         <f>IF(SUM(B4:$K$4)=0,"",SUMPRODUCT(B19:$K$19,B4:$K$4)/SUM(B4:$K$4))</f>
-      </c>
-      <c r="I24" s="7" t="str">
+        <v>0.58832210775160532</v>
+      </c>
+      <c r="I24" s="7">
         <f>IF(SUM(E4:$K$4)=0,"",SUMPRODUCT(E19:$K$19,E4:$K$4)/SUM(E4:$K$4))</f>
-      </c>
-      <c r="J24" s="7" t="str">
+        <v>0.57803075291541228</v>
+      </c>
+      <c r="J24" s="7">
         <f>IF(SUM(G4:$K$4)=0,"",SUMPRODUCT(G19:$K$19,G4:$K$4)/SUM(G4:$K$4))</f>
-      </c>
-      <c r="K24" s="7" t="str">
+        <v>0.58393096998417648</v>
+      </c>
+      <c r="K24" s="7">
         <f>IF(SUM(I4:$K$4)=0, "", SUMPRODUCT(I19:$K$19,I4:$K$4)/SUM(I4:$K$4))</f>
+        <v>0.57250537560002979</v>
       </c>
       <c r="L24" s="7">
         <f>L19</f>
+        <v>0.60436152207628402</v>
       </c>
       <c r="M24" s="22">
         <f>MAX(K24:L24)</f>
+        <v>0.60436152207628402</v>
       </c>
       <c r="N24" s="22">
         <f>MIN(H24:L24)</f>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.57250537560002979</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="9" t="str">
+      <c r="H25" s="9">
         <f>IF(ISERROR(AVERAGEIF(B14:$L14,"&gt;0")),"",AVERAGEIF(B14:$L14,"&gt;0"))</f>
-      </c>
-      <c r="I25" s="9" t="str">
+        <v>23.774836906122676</v>
+      </c>
+      <c r="I25" s="9">
         <f>IF(ISERROR(AVERAGEIF(E14:$L14,"&gt;0")),"",AVERAGEIF(E14:$L14,"&gt;0"))</f>
-      </c>
-      <c r="J25" s="9" t="str">
+        <v>25.734224275828367</v>
+      </c>
+      <c r="J25" s="9">
         <f>IF(ISERROR(AVERAGEIF(G14:$L14,"&gt;0")),"",AVERAGEIF(G14:$L14,"&gt;0"))</f>
-      </c>
-      <c r="K25" s="9" t="str">
+        <v>28.779804768004198</v>
+      </c>
+      <c r="K25" s="9">
         <f>IF(ISERROR(AVERAGEIF(I14:$L14,"&gt;0")),"",AVERAGEIF(I14:$L14,"&gt;0"))</f>
+        <v>27.658044717167506</v>
       </c>
       <c r="L25" s="9">
         <f>L14</f>
+        <v>26.147041508937278</v>
       </c>
       <c r="M25" s="1">
         <f>MAX(K25:L25)</f>
+        <v>27.658044717167506</v>
       </c>
       <c r="N25" s="1">
         <f>MIN(H25:L25)</f>
+        <v>23.774836906122676</v>
       </c>
     </row>
   </sheetData>
@@ -2570,411 +2771,523 @@
       <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="6" customWidth="1"/>
-    <col min="2" max="11" width="13.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="20.7109375" style="6" customWidth="1"/>
+    <col min="2" max="11" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="str">
         <f>'Profit &amp; Loss'!A1</f>
+        <v>ADANI PORTS &amp; SPECIAL ECONOMIC ZONE LTD</v>
       </c>
       <c r="E1" t="str">
         <f>UPDATE</f>
+        <v/>
       </c>
       <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16">
         <f>'Data Sheet'!B41</f>
+        <v>44926</v>
       </c>
       <c r="C3" s="16">
         <f>'Data Sheet'!C41</f>
+        <v>45016</v>
       </c>
       <c r="D3" s="16">
         <f>'Data Sheet'!D41</f>
+        <v>45107</v>
       </c>
       <c r="E3" s="16">
         <f>'Data Sheet'!E41</f>
+        <v>45199</v>
       </c>
       <c r="F3" s="16">
         <f>'Data Sheet'!F41</f>
+        <v>45291</v>
       </c>
       <c r="G3" s="16">
         <f>'Data Sheet'!G41</f>
+        <v>45382</v>
       </c>
       <c r="H3" s="16">
         <f>'Data Sheet'!H41</f>
+        <v>45473</v>
       </c>
       <c r="I3" s="16">
         <f>'Data Sheet'!I41</f>
+        <v>45565</v>
       </c>
       <c r="J3" s="16">
         <f>'Data Sheet'!J41</f>
+        <v>45657</v>
       </c>
       <c r="K3" s="16">
         <f>'Data Sheet'!K41</f>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
         <f>'Data Sheet'!B42</f>
+        <v>4786.17</v>
       </c>
       <c r="C4" s="1">
         <f>'Data Sheet'!C42</f>
+        <v>5796.85</v>
       </c>
       <c r="D4" s="1">
         <f>'Data Sheet'!D42</f>
+        <v>6247.55</v>
       </c>
       <c r="E4" s="1">
         <f>'Data Sheet'!E42</f>
+        <v>6646.41</v>
       </c>
       <c r="F4" s="1">
         <f>'Data Sheet'!F42</f>
+        <v>6920.1</v>
       </c>
       <c r="G4" s="1">
         <f>'Data Sheet'!G42</f>
+        <v>6896.5</v>
       </c>
       <c r="H4" s="1">
         <f>'Data Sheet'!H42</f>
+        <v>7559.59</v>
       </c>
       <c r="I4" s="1">
         <f>'Data Sheet'!I42</f>
+        <v>7067.02</v>
       </c>
       <c r="J4" s="1">
         <f>'Data Sheet'!J42</f>
+        <v>7963.55</v>
       </c>
       <c r="K4" s="1">
         <f>'Data Sheet'!K42</f>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>8488.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="9">
         <f>'Data Sheet'!B43</f>
+        <v>2089.67</v>
       </c>
       <c r="C5" s="9">
         <f>'Data Sheet'!C43</f>
+        <v>2526.17</v>
       </c>
       <c r="D5" s="9">
         <f>'Data Sheet'!D43</f>
+        <v>2558.2199999999998</v>
       </c>
       <c r="E5" s="9">
         <f>'Data Sheet'!E43</f>
+        <v>2982.43</v>
       </c>
       <c r="F5" s="9">
         <f>'Data Sheet'!F43</f>
+        <v>2724.42</v>
       </c>
       <c r="G5" s="9">
         <f>'Data Sheet'!G43</f>
+        <v>2887.39</v>
       </c>
       <c r="H5" s="9">
         <f>'Data Sheet'!H43</f>
+        <v>2820.17</v>
       </c>
       <c r="I5" s="9">
         <f>'Data Sheet'!I43</f>
+        <v>2831.75</v>
       </c>
       <c r="J5" s="9">
         <f>'Data Sheet'!J43</f>
+        <v>3161.49</v>
       </c>
       <c r="K5" s="9">
         <f>'Data Sheet'!K43</f>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3482.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
         <f>'Data Sheet'!B50</f>
+        <v>2696.5</v>
       </c>
       <c r="C6" s="1">
         <f>'Data Sheet'!C50</f>
+        <v>3270.68</v>
       </c>
       <c r="D6" s="1">
         <f>'Data Sheet'!D50</f>
+        <v>3689.33</v>
       </c>
       <c r="E6" s="1">
         <f>'Data Sheet'!E50</f>
+        <v>3663.98</v>
       </c>
       <c r="F6" s="1">
         <f>'Data Sheet'!F50</f>
+        <v>4195.68</v>
       </c>
       <c r="G6" s="1">
         <f>'Data Sheet'!G50</f>
+        <v>4009.11</v>
       </c>
       <c r="H6" s="1">
         <f>'Data Sheet'!H50</f>
+        <v>4739.42</v>
       </c>
       <c r="I6" s="1">
         <f>'Data Sheet'!I50</f>
+        <v>4235.2700000000004</v>
       </c>
       <c r="J6" s="1">
         <f>'Data Sheet'!J50</f>
+        <v>4802.0600000000004</v>
       </c>
       <c r="K6" s="1">
         <f>'Data Sheet'!K50</f>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5005.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="9">
         <f>'Data Sheet'!B44</f>
+        <v>284.91000000000003</v>
       </c>
       <c r="C7" s="9">
         <f>'Data Sheet'!C44</f>
+        <v>-884.53</v>
       </c>
       <c r="D7" s="9">
         <f>'Data Sheet'!D44</f>
+        <v>383.68</v>
       </c>
       <c r="E7" s="9">
         <f>'Data Sheet'!E44</f>
+        <v>351.27</v>
       </c>
       <c r="F7" s="9">
         <f>'Data Sheet'!F44</f>
+        <v>506.85</v>
       </c>
       <c r="G7" s="9">
         <f>'Data Sheet'!G44</f>
+        <v>-70.260000000000005</v>
       </c>
       <c r="H7" s="9">
         <f>'Data Sheet'!H44</f>
+        <v>349.16</v>
       </c>
       <c r="I7" s="9">
         <f>'Data Sheet'!I44</f>
+        <v>253.58</v>
       </c>
       <c r="J7" s="9">
         <f>'Data Sheet'!J44</f>
+        <v>246.85</v>
       </c>
       <c r="K7" s="9">
         <f>'Data Sheet'!K44</f>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>425.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="9">
         <f>'Data Sheet'!B45</f>
+        <v>883.63</v>
       </c>
       <c r="C8" s="9">
         <f>'Data Sheet'!C45</f>
+        <v>846.36</v>
       </c>
       <c r="D8" s="9">
         <f>'Data Sheet'!D45</f>
+        <v>949.58</v>
       </c>
       <c r="E8" s="9">
         <f>'Data Sheet'!E45</f>
+        <v>974.47</v>
       </c>
       <c r="F8" s="9">
         <f>'Data Sheet'!F45</f>
+        <v>985.32</v>
       </c>
       <c r="G8" s="9">
         <f>'Data Sheet'!G45</f>
+        <v>979.09</v>
       </c>
       <c r="H8" s="9">
         <f>'Data Sheet'!H45</f>
+        <v>1011.87</v>
       </c>
       <c r="I8" s="9">
         <f>'Data Sheet'!I45</f>
+        <v>1076.57</v>
       </c>
       <c r="J8" s="9">
         <f>'Data Sheet'!J45</f>
+        <v>1105.76</v>
       </c>
       <c r="K8" s="9">
         <f>'Data Sheet'!K45</f>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1184.73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9">
         <f>'Data Sheet'!B46</f>
+        <v>533.88</v>
       </c>
       <c r="C9" s="9">
         <f>'Data Sheet'!C46</f>
+        <v>622.55999999999995</v>
       </c>
       <c r="D9" s="9">
         <f>'Data Sheet'!D46</f>
+        <v>632.69000000000005</v>
       </c>
       <c r="E9" s="9">
         <f>'Data Sheet'!E46</f>
+        <v>520.1</v>
       </c>
       <c r="F9" s="9">
         <f>'Data Sheet'!F46</f>
+        <v>975.88</v>
       </c>
       <c r="G9" s="9">
         <f>'Data Sheet'!G46</f>
+        <v>618.78</v>
       </c>
       <c r="H9" s="9">
         <f>'Data Sheet'!H46</f>
+        <v>484.06</v>
       </c>
       <c r="I9" s="9">
         <f>'Data Sheet'!I46</f>
+        <v>527.11</v>
       </c>
       <c r="J9" s="9">
         <f>'Data Sheet'!J46</f>
+        <v>923.28</v>
       </c>
       <c r="K9" s="9">
         <f>'Data Sheet'!K46</f>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>714.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="9">
         <f>'Data Sheet'!B47</f>
+        <v>1563.9</v>
       </c>
       <c r="C10" s="9">
         <f>'Data Sheet'!C47</f>
+        <v>917.23</v>
       </c>
       <c r="D10" s="9">
         <f>'Data Sheet'!D47</f>
+        <v>2490.7399999999998</v>
       </c>
       <c r="E10" s="9">
         <f>'Data Sheet'!E47</f>
+        <v>2520.6799999999998</v>
       </c>
       <c r="F10" s="9">
         <f>'Data Sheet'!F47</f>
+        <v>2741.33</v>
       </c>
       <c r="G10" s="9">
         <f>'Data Sheet'!G47</f>
+        <v>2340.98</v>
       </c>
       <c r="H10" s="9">
         <f>'Data Sheet'!H47</f>
+        <v>3592.65</v>
       </c>
       <c r="I10" s="9">
         <f>'Data Sheet'!I47</f>
+        <v>2885.17</v>
       </c>
       <c r="J10" s="9">
         <f>'Data Sheet'!J47</f>
+        <v>3019.87</v>
       </c>
       <c r="K10" s="9">
         <f>'Data Sheet'!K47</f>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3531.93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="9">
         <f>'Data Sheet'!B48</f>
+        <v>227.39</v>
       </c>
       <c r="C11" s="9">
         <f>'Data Sheet'!C48</f>
+        <v>-221.84</v>
       </c>
       <c r="D11" s="9">
         <f>'Data Sheet'!D48</f>
+        <v>371.36</v>
       </c>
       <c r="E11" s="9">
         <f>'Data Sheet'!E48</f>
+        <v>759.05</v>
       </c>
       <c r="F11" s="9">
         <f>'Data Sheet'!F48</f>
+        <v>533.12</v>
       </c>
       <c r="G11" s="9">
         <f>'Data Sheet'!G48</f>
+        <v>326.20999999999998</v>
       </c>
       <c r="H11" s="9">
         <f>'Data Sheet'!H48</f>
+        <v>485.42</v>
       </c>
       <c r="I11" s="9">
         <f>'Data Sheet'!I48</f>
+        <v>472.63</v>
       </c>
       <c r="J11" s="9">
         <f>'Data Sheet'!J48</f>
+        <v>501.48</v>
       </c>
       <c r="K11" s="9">
         <f>'Data Sheet'!K48</f>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>508.83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1">
         <f>'Data Sheet'!B49</f>
+        <v>1315.54</v>
       </c>
       <c r="C12" s="1">
         <f>'Data Sheet'!C49</f>
+        <v>1157.55</v>
       </c>
       <c r="D12" s="1">
         <f>'Data Sheet'!D49</f>
+        <v>2114.7199999999998</v>
       </c>
       <c r="E12" s="1">
         <f>'Data Sheet'!E49</f>
+        <v>1747.85</v>
       </c>
       <c r="F12" s="1">
         <f>'Data Sheet'!F49</f>
+        <v>2208.41</v>
       </c>
       <c r="G12" s="1">
         <f>'Data Sheet'!G49</f>
+        <v>2039.66</v>
       </c>
       <c r="H12" s="1">
         <f>'Data Sheet'!H49</f>
+        <v>3112.83</v>
       </c>
       <c r="I12" s="1">
         <f>'Data Sheet'!I49</f>
+        <v>2445</v>
       </c>
       <c r="J12" s="1">
         <f>'Data Sheet'!J49</f>
+        <v>2520.2600000000002</v>
       </c>
       <c r="K12" s="1">
         <f>'Data Sheet'!K49</f>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3014.22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="14" t="str">
+      <c r="B14" s="14">
         <f>IF(B4&gt;0,B6/B4,"")</f>
-      </c>
-      <c r="C14" s="14" t="str">
+        <v>0.56339411262032058</v>
+      </c>
+      <c r="C14" s="14">
         <f t="shared" ref="C14:K14" si="0">IF(C4&gt;0,C6/C4,"")</f>
-      </c>
-      <c r="D14" s="14" t="str">
+        <v>0.56421677290252459</v>
+      </c>
+      <c r="D14" s="14">
         <f t="shared" si="0"/>
-      </c>
-      <c r="E14" s="14" t="str">
+        <v>0.59052428551992375</v>
+      </c>
+      <c r="E14" s="14">
         <f t="shared" si="0"/>
-      </c>
-      <c r="F14" s="14" t="str">
+        <v>0.55127204009382513</v>
+      </c>
+      <c r="F14" s="14">
         <f t="shared" si="0"/>
-      </c>
-      <c r="G14" s="14" t="str">
+        <v>0.60630337711882776</v>
+      </c>
+      <c r="G14" s="14">
         <f t="shared" si="0"/>
-      </c>
-      <c r="H14" s="14" t="str">
+        <v>0.58132530993982456</v>
+      </c>
+      <c r="H14" s="14">
         <f t="shared" si="0"/>
-      </c>
-      <c r="I14" s="14" t="str">
+        <v>0.62694140819806365</v>
+      </c>
+      <c r="I14" s="14">
         <f t="shared" si="0"/>
-      </c>
-      <c r="J14" s="14" t="str">
+        <v>0.59930069534259134</v>
+      </c>
+      <c r="J14" s="14">
         <f t="shared" si="0"/>
-      </c>
-      <c r="K14" s="14" t="str">
+        <v>0.60300494126363247</v>
+      </c>
+      <c r="K14" s="14">
         <f t="shared" si="0"/>
-      </c>
-    </row>
-    <row r="22" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+        <v>0.58973851496859253</v>
+      </c>
+    </row>
+    <row r="22" s="30" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -3003,20 +3316,22 @@
       <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="11" customWidth="1"/>
-    <col min="3" max="11" width="15.5" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="22.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="11" customWidth="1"/>
+    <col min="3" max="11" width="15.42578125" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="str">
         <f>'Profit &amp; Loss'!A1</f>
+        <v>ADANI PORTS &amp; SPECIAL ECONOMIC ZONE LTD</v>
       </c>
       <c r="E1" t="str">
         <f>UPDATE</f>
+        <v/>
       </c>
       <c r="G1"/>
       <c r="J1" s="4" t="s">
@@ -3024,221 +3339,281 @@
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16">
         <f>'Data Sheet'!B56</f>
+        <v>42460</v>
       </c>
       <c r="C3" s="16">
         <f>'Data Sheet'!C56</f>
+        <v>42825</v>
       </c>
       <c r="D3" s="16">
         <f>'Data Sheet'!D56</f>
+        <v>43190</v>
       </c>
       <c r="E3" s="16">
         <f>'Data Sheet'!E56</f>
+        <v>43555</v>
       </c>
       <c r="F3" s="16">
         <f>'Data Sheet'!F56</f>
+        <v>43921</v>
       </c>
       <c r="G3" s="16">
         <f>'Data Sheet'!G56</f>
+        <v>44286</v>
       </c>
       <c r="H3" s="16">
         <f>'Data Sheet'!H56</f>
+        <v>44651</v>
       </c>
       <c r="I3" s="16">
         <f>'Data Sheet'!I56</f>
+        <v>45016</v>
       </c>
       <c r="J3" s="16">
         <f>'Data Sheet'!J56</f>
+        <v>45382</v>
       </c>
       <c r="K3" s="16">
         <f>'Data Sheet'!K56</f>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="19">
         <f>'Data Sheet'!B57</f>
+        <v>414.19</v>
       </c>
       <c r="C4" s="19">
         <f>'Data Sheet'!C57</f>
+        <v>414.19</v>
       </c>
       <c r="D4" s="19">
         <f>'Data Sheet'!D57</f>
+        <v>414.19</v>
       </c>
       <c r="E4" s="19">
         <f>'Data Sheet'!E57</f>
+        <v>414.19</v>
       </c>
       <c r="F4" s="19">
         <f>'Data Sheet'!F57</f>
+        <v>406.35</v>
       </c>
       <c r="G4" s="19">
         <f>'Data Sheet'!G57</f>
+        <v>406.35</v>
       </c>
       <c r="H4" s="19">
         <f>'Data Sheet'!H57</f>
+        <v>422.47</v>
       </c>
       <c r="I4" s="19">
         <f>'Data Sheet'!I57</f>
+        <v>432.03</v>
       </c>
       <c r="J4" s="19">
         <f>'Data Sheet'!J57</f>
+        <v>432.03</v>
       </c>
       <c r="K4" s="19">
         <f>'Data Sheet'!K57</f>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>432.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="19">
         <f>'Data Sheet'!B58</f>
+        <v>13091.3</v>
       </c>
       <c r="C5" s="19">
         <f>'Data Sheet'!C58</f>
+        <v>17111.79</v>
       </c>
       <c r="D5" s="19">
         <f>'Data Sheet'!D58</f>
+        <v>20488.759999999998</v>
       </c>
       <c r="E5" s="19">
         <f>'Data Sheet'!E58</f>
+        <v>23958.13</v>
       </c>
       <c r="F5" s="19">
         <f>'Data Sheet'!F58</f>
+        <v>25050.61</v>
       </c>
       <c r="G5" s="19">
         <f>'Data Sheet'!G58</f>
+        <v>30035.38</v>
       </c>
       <c r="H5" s="19">
         <f>'Data Sheet'!H58</f>
+        <v>41399.22</v>
       </c>
       <c r="I5" s="19">
         <f>'Data Sheet'!I58</f>
+        <v>44957.36</v>
       </c>
       <c r="J5" s="19">
         <f>'Data Sheet'!J58</f>
+        <v>52346.21</v>
       </c>
       <c r="K5" s="19">
         <f>'Data Sheet'!K58</f>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>61836.83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B6" s="19">
         <f>'Data Sheet'!B59</f>
+        <v>22341.53</v>
       </c>
       <c r="C6" s="19">
         <f>'Data Sheet'!C59</f>
+        <v>22214.26</v>
       </c>
       <c r="D6" s="19">
         <f>'Data Sheet'!D59</f>
+        <v>22370.04</v>
       </c>
       <c r="E6" s="19">
         <f>'Data Sheet'!E59</f>
+        <v>27711.54</v>
       </c>
       <c r="F6" s="19">
         <f>'Data Sheet'!F59</f>
+        <v>30242.32</v>
       </c>
       <c r="G6" s="19">
         <f>'Data Sheet'!G59</f>
+        <v>35855.33</v>
       </c>
       <c r="H6" s="19">
         <f>'Data Sheet'!H59</f>
+        <v>47934.75</v>
       </c>
       <c r="I6" s="19">
         <f>'Data Sheet'!I59</f>
+        <v>53434.22</v>
       </c>
       <c r="J6" s="19">
         <f>'Data Sheet'!J59</f>
+        <v>49470.239999999998</v>
       </c>
       <c r="K6" s="19">
         <f>'Data Sheet'!K59</f>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>51620.73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
       <c r="B7" s="19">
         <f>'Data Sheet'!B60</f>
+        <v>2537.83</v>
       </c>
       <c r="C7" s="19">
         <f>'Data Sheet'!C60</f>
+        <v>3629.13</v>
       </c>
       <c r="D7" s="19">
         <f>'Data Sheet'!D60</f>
+        <v>3959.73</v>
       </c>
       <c r="E7" s="19">
         <f>'Data Sheet'!E60</f>
+        <v>4227.57</v>
       </c>
       <c r="F7" s="19">
         <f>'Data Sheet'!F60</f>
+        <v>6217.42</v>
       </c>
       <c r="G7" s="19">
         <f>'Data Sheet'!G60</f>
+        <v>8284.8700000000008</v>
       </c>
       <c r="H7" s="19">
         <f>'Data Sheet'!H60</f>
+        <v>8571.5499999999993</v>
       </c>
       <c r="I7" s="19">
         <f>'Data Sheet'!I60</f>
+        <v>13739.58</v>
       </c>
       <c r="J7" s="19">
         <f>'Data Sheet'!J60</f>
+        <v>14750.72</v>
       </c>
       <c r="K7" s="19">
         <f>'Data Sheet'!K60</f>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>19553.060000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="20">
         <f>'Data Sheet'!B61</f>
+        <v>38384.85</v>
       </c>
       <c r="C8" s="20">
         <f>'Data Sheet'!C61</f>
+        <v>43369.37</v>
       </c>
       <c r="D8" s="20">
         <f>'Data Sheet'!D61</f>
+        <v>47232.72</v>
       </c>
       <c r="E8" s="20">
         <f>'Data Sheet'!E61</f>
+        <v>56311.43</v>
       </c>
       <c r="F8" s="20">
         <f>'Data Sheet'!F61</f>
+        <v>61916.7</v>
       </c>
       <c r="G8" s="20">
         <f>'Data Sheet'!G61</f>
+        <v>74581.929999999993</v>
       </c>
       <c r="H8" s="20">
         <f>'Data Sheet'!H61</f>
+        <v>98327.99</v>
       </c>
       <c r="I8" s="20">
         <f>'Data Sheet'!I61</f>
+        <v>112563.19</v>
       </c>
       <c r="J8" s="20">
         <f>'Data Sheet'!J61</f>
+        <v>116999.2</v>
       </c>
       <c r="K8" s="20">
         <f>'Data Sheet'!K61</f>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>133442.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -3250,182 +3625,232 @@
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="19">
         <f>'Data Sheet'!B62</f>
+        <v>20883.22</v>
       </c>
       <c r="C10" s="19">
         <f>'Data Sheet'!C62</f>
+        <v>21053.5</v>
       </c>
       <c r="D10" s="19">
         <f>'Data Sheet'!D62</f>
+        <v>22670.01</v>
       </c>
       <c r="E10" s="19">
         <f>'Data Sheet'!E62</f>
+        <v>28121.42</v>
       </c>
       <c r="F10" s="19">
         <f>'Data Sheet'!F62</f>
+        <v>32714.51</v>
       </c>
       <c r="G10" s="19">
         <f>'Data Sheet'!G62</f>
+        <v>48290.96</v>
       </c>
       <c r="H10" s="19">
         <f>'Data Sheet'!H62</f>
+        <v>62552.92</v>
       </c>
       <c r="I10" s="19">
         <f>'Data Sheet'!I62</f>
+        <v>72223.73</v>
       </c>
       <c r="J10" s="19">
         <f>'Data Sheet'!J62</f>
+        <v>75147.81</v>
       </c>
       <c r="K10" s="19">
         <f>'Data Sheet'!K62</f>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>89616.320000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="19">
         <f>'Data Sheet'!B63</f>
+        <v>1966.76</v>
       </c>
       <c r="C11" s="19">
         <f>'Data Sheet'!C63</f>
+        <v>4513.97</v>
       </c>
       <c r="D11" s="19">
         <f>'Data Sheet'!D63</f>
+        <v>4545.46</v>
       </c>
       <c r="E11" s="19">
         <f>'Data Sheet'!E63</f>
+        <v>4483.4799999999996</v>
       </c>
       <c r="F11" s="19">
         <f>'Data Sheet'!F63</f>
+        <v>3216.33</v>
       </c>
       <c r="G11" s="19">
         <f>'Data Sheet'!G63</f>
+        <v>3697.13</v>
       </c>
       <c r="H11" s="19">
         <f>'Data Sheet'!H63</f>
+        <v>4022.9</v>
       </c>
       <c r="I11" s="19">
         <f>'Data Sheet'!I63</f>
+        <v>6636.77</v>
       </c>
       <c r="J11" s="19">
         <f>'Data Sheet'!J63</f>
+        <v>10936.09</v>
       </c>
       <c r="K11" s="19">
         <f>'Data Sheet'!K63</f>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11706.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="19">
         <f>'Data Sheet'!B64</f>
+        <v>545.17999999999995</v>
       </c>
       <c r="C12" s="19">
         <f>'Data Sheet'!C64</f>
+        <v>1161.3599999999999</v>
       </c>
       <c r="D12" s="19">
         <f>'Data Sheet'!D64</f>
+        <v>1078.92</v>
       </c>
       <c r="E12" s="19">
         <f>'Data Sheet'!E64</f>
+        <v>782.3</v>
       </c>
       <c r="F12" s="19">
         <f>'Data Sheet'!F64</f>
+        <v>1178</v>
       </c>
       <c r="G12" s="19">
         <f>'Data Sheet'!G64</f>
+        <v>2236.15</v>
       </c>
       <c r="H12" s="19">
         <f>'Data Sheet'!H64</f>
+        <v>3160.74</v>
       </c>
       <c r="I12" s="19">
         <f>'Data Sheet'!I64</f>
+        <v>7431.65</v>
       </c>
       <c r="J12" s="19">
         <f>'Data Sheet'!J64</f>
+        <v>4288.66</v>
       </c>
       <c r="K12" s="19">
         <f>'Data Sheet'!K64</f>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4659.45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>73</v>
       </c>
       <c r="B13" s="19">
         <f>'Data Sheet'!B65</f>
+        <v>14989.69</v>
       </c>
       <c r="C13" s="19">
         <f>'Data Sheet'!C65</f>
+        <v>16640.54</v>
       </c>
       <c r="D13" s="19">
         <f>'Data Sheet'!D65</f>
+        <v>18938.330000000002</v>
       </c>
       <c r="E13" s="19">
         <f>'Data Sheet'!E65</f>
+        <v>22924.23</v>
       </c>
       <c r="F13" s="19">
         <f>'Data Sheet'!F65</f>
+        <v>24807.86</v>
       </c>
       <c r="G13" s="19">
         <f>'Data Sheet'!G65</f>
+        <v>20357.689999999999</v>
       </c>
       <c r="H13" s="19">
         <f>'Data Sheet'!H65</f>
+        <v>28591.43</v>
       </c>
       <c r="I13" s="19">
         <f>'Data Sheet'!I65</f>
+        <v>26271.040000000001</v>
       </c>
       <c r="J13" s="19">
         <f>'Data Sheet'!J65</f>
+        <v>26626.639999999999</v>
       </c>
       <c r="K13" s="19">
         <f>'Data Sheet'!K65</f>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>27460.78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="19">
         <f>'Data Sheet'!B66</f>
+        <v>38384.85</v>
       </c>
       <c r="C14" s="19">
         <f>'Data Sheet'!C66</f>
+        <v>43369.37</v>
       </c>
       <c r="D14" s="19">
         <f>'Data Sheet'!D66</f>
+        <v>47232.72</v>
       </c>
       <c r="E14" s="19">
         <f>'Data Sheet'!E66</f>
+        <v>56311.43</v>
       </c>
       <c r="F14" s="19">
         <f>'Data Sheet'!F66</f>
+        <v>61916.7</v>
       </c>
       <c r="G14" s="19">
         <f>'Data Sheet'!G66</f>
+        <v>74581.929999999993</v>
       </c>
       <c r="H14" s="19">
         <f>'Data Sheet'!H66</f>
+        <v>98327.99</v>
       </c>
       <c r="I14" s="19">
         <f>'Data Sheet'!I66</f>
+        <v>112563.19</v>
       </c>
       <c r="J14" s="19">
         <f>'Data Sheet'!J66</f>
+        <v>116999.2</v>
       </c>
       <c r="K14" s="19">
         <f>'Data Sheet'!K66</f>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>133442.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -3438,250 +3863,319 @@
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="21">
         <f>B13-B7</f>
+        <v>12451.86</v>
       </c>
       <c r="C16" s="21">
         <f t="shared" ref="C16:K16" si="0">C13-C7</f>
+        <v>13011.41</v>
       </c>
       <c r="D16" s="21">
         <f t="shared" si="0"/>
+        <v>14978.600000000002</v>
       </c>
       <c r="E16" s="21">
         <f t="shared" si="0"/>
+        <v>18696.66</v>
       </c>
       <c r="F16" s="21">
         <f t="shared" si="0"/>
+        <v>18590.440000000002</v>
       </c>
       <c r="G16" s="21">
         <f t="shared" si="0"/>
+        <v>12072.819999999998</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" si="0"/>
+        <v>20019.88</v>
       </c>
       <c r="I16" s="21">
         <f t="shared" si="0"/>
+        <v>12531.460000000001</v>
       </c>
       <c r="J16" s="21">
         <f t="shared" si="0"/>
+        <v>11875.92</v>
       </c>
       <c r="K16" s="21">
         <f t="shared" si="0"/>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>7907.7199999999975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="21">
         <f>'Data Sheet'!B67</f>
+        <v>2436.09</v>
       </c>
       <c r="C17" s="21">
         <f>'Data Sheet'!C67</f>
+        <v>2692.99</v>
       </c>
       <c r="D17" s="21">
         <f>'Data Sheet'!D67</f>
+        <v>4309.91</v>
       </c>
       <c r="E17" s="21">
         <f>'Data Sheet'!E67</f>
+        <v>2789.66</v>
       </c>
       <c r="F17" s="21">
         <f>'Data Sheet'!F67</f>
+        <v>3202.14</v>
       </c>
       <c r="G17" s="21">
         <f>'Data Sheet'!G67</f>
+        <v>2925.71</v>
       </c>
       <c r="H17" s="21">
         <f>'Data Sheet'!H67</f>
+        <v>2521.14</v>
       </c>
       <c r="I17" s="21">
         <f>'Data Sheet'!I67</f>
+        <v>3957.07</v>
       </c>
       <c r="J17" s="21">
         <f>'Data Sheet'!J67</f>
+        <v>3666.94</v>
       </c>
       <c r="K17" s="21">
         <f>'Data Sheet'!K67</f>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4432.3599999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="21">
         <f>'Data Sheet'!B68</f>
+        <v>211.89</v>
       </c>
       <c r="C18" s="21">
         <f>'Data Sheet'!C68</f>
+        <v>657.09</v>
       </c>
       <c r="D18" s="21">
         <f>'Data Sheet'!D68</f>
+        <v>520.29</v>
       </c>
       <c r="E18" s="21">
         <f>'Data Sheet'!E68</f>
+        <v>806.68</v>
       </c>
       <c r="F18" s="21">
         <f>'Data Sheet'!F68</f>
+        <v>288.27999999999997</v>
       </c>
       <c r="G18" s="21">
         <f>'Data Sheet'!G68</f>
+        <v>991.85</v>
       </c>
       <c r="H18" s="21">
         <f>'Data Sheet'!H68</f>
+        <v>395.64</v>
       </c>
       <c r="I18" s="21">
         <f>'Data Sheet'!I68</f>
+        <v>451.97</v>
       </c>
       <c r="J18" s="21">
         <f>'Data Sheet'!J68</f>
+        <v>437.51</v>
       </c>
       <c r="K18" s="21">
         <f>'Data Sheet'!K68</f>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>521.79999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="5">
         <f>IF('Profit &amp; Loss'!B4&gt;0,'Balance Sheet'!B17/('Profit &amp; Loss'!B4/365),0)</f>
+        <v>125.0832225528054</v>
       </c>
       <c r="C20" s="5">
         <f>IF('Profit &amp; Loss'!C4&gt;0,'Balance Sheet'!C17/('Profit &amp; Loss'!C4/365),0)</f>
+        <v>116.47121520022276</v>
       </c>
       <c r="D20" s="5">
         <f>IF('Profit &amp; Loss'!D4&gt;0,'Balance Sheet'!D17/('Profit &amp; Loss'!D4/365),0)</f>
+        <v>138.93161770420457</v>
       </c>
       <c r="E20" s="5">
         <f>IF('Profit &amp; Loss'!E4&gt;0,'Balance Sheet'!E17/('Profit &amp; Loss'!E4/365),0)</f>
+        <v>93.197701877452985</v>
       </c>
       <c r="F20" s="5">
         <f>IF('Profit &amp; Loss'!F4&gt;0,'Balance Sheet'!F17/('Profit &amp; Loss'!F4/365),0)</f>
+        <v>98.439670615940116</v>
       </c>
       <c r="G20" s="5">
         <f>IF('Profit &amp; Loss'!G4&gt;0,'Balance Sheet'!G17/('Profit &amp; Loss'!G4/365),0)</f>
+        <v>85.093082648052516</v>
       </c>
       <c r="H20" s="5">
         <f>IF('Profit &amp; Loss'!H4&gt;0,'Balance Sheet'!H17/('Profit &amp; Loss'!H4/365),0)</f>
+        <v>53.754739674941973</v>
       </c>
       <c r="I20" s="5">
         <f>IF('Profit &amp; Loss'!I4&gt;0,'Balance Sheet'!I17/('Profit &amp; Loss'!I4/365),0)</f>
+        <v>69.26610320109765</v>
       </c>
       <c r="J20" s="5">
         <f>IF('Profit &amp; Loss'!J4&gt;0,'Balance Sheet'!J17/('Profit &amp; Loss'!J4/365),0)</f>
+        <v>50.108762227373745</v>
       </c>
       <c r="K20" s="5">
         <f>IF('Profit &amp; Loss'!K4&gt;0,'Balance Sheet'!K17/('Profit &amp; Loss'!K4/365),0)</f>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>53.085935410707606</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="5">
         <f>IF('Balance Sheet'!B18&gt;0,'Profit &amp; Loss'!B4/'Balance Sheet'!B18,0)</f>
+        <v>33.548775307942797</v>
       </c>
       <c r="C21" s="5">
         <f>IF('Balance Sheet'!C18&gt;0,'Profit &amp; Loss'!C4/'Balance Sheet'!C18,0)</f>
+        <v>12.843522196350577</v>
       </c>
       <c r="D21" s="5">
         <f>IF('Balance Sheet'!D18&gt;0,'Profit &amp; Loss'!D4/'Balance Sheet'!D18,0)</f>
+        <v>21.762786138499681</v>
       </c>
       <c r="E21" s="5">
         <f>IF('Balance Sheet'!E18&gt;0,'Profit &amp; Loss'!E4/'Balance Sheet'!E18,0)</f>
+        <v>13.543710021321964</v>
       </c>
       <c r="F21" s="5">
         <f>IF('Balance Sheet'!F18&gt;0,'Profit &amp; Loss'!F4/'Balance Sheet'!F18,0)</f>
+        <v>41.185895657000138</v>
       </c>
       <c r="G21" s="5">
         <f>IF('Balance Sheet'!G18&gt;0,'Profit &amp; Loss'!G4/'Balance Sheet'!G18,0)</f>
+        <v>12.652719665271967</v>
       </c>
       <c r="H21" s="5">
         <f>IF('Balance Sheet'!H18&gt;0,'Profit &amp; Loss'!H4/'Balance Sheet'!H18,0)</f>
+        <v>43.26860277019513</v>
       </c>
       <c r="I21" s="5">
         <f>IF('Balance Sheet'!I18&gt;0,'Profit &amp; Loss'!I4/'Balance Sheet'!I18,0)</f>
+        <v>46.135606345553903</v>
       </c>
       <c r="J21" s="5">
         <f>IF('Balance Sheet'!J18&gt;0,'Profit &amp; Loss'!J4/'Balance Sheet'!J18,0)</f>
+        <v>61.05131311284314</v>
       </c>
       <c r="K21" s="5">
         <f>IF('Balance Sheet'!K18&gt;0,'Profit &amp; Loss'!K4/'Balance Sheet'!K18,0)</f>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>58.404235339210437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="14" t="str">
+      <c r="B23" s="14">
         <f>IF(SUM('Balance Sheet'!B4:B5)&gt;0,'Profit &amp; Loss'!B12/SUM('Balance Sheet'!B4:B5),"")</f>
-      </c>
-      <c r="C23" s="14" t="str">
+        <v>0.21451720744674943</v>
+      </c>
+      <c r="C23" s="14">
         <f>IF(SUM('Balance Sheet'!C4:C5)&gt;0,'Profit &amp; Loss'!C12/SUM('Balance Sheet'!C4:C5),"")</f>
-      </c>
-      <c r="D23" s="14" t="str">
+        <v>0.2231840958394338</v>
+      </c>
+      <c r="D23" s="14">
         <f>IF(SUM('Balance Sheet'!D4:D5)&gt;0,'Profit &amp; Loss'!D12/SUM('Balance Sheet'!D4:D5),"")</f>
-      </c>
-      <c r="E23" s="14" t="str">
+        <v>0.17574648554390651</v>
+      </c>
+      <c r="E23" s="14">
         <f>IF(SUM('Balance Sheet'!E4:E5)&gt;0,'Profit &amp; Loss'!E12/SUM('Balance Sheet'!E4:E5),"")</f>
-      </c>
-      <c r="F23" s="14" t="str">
+        <v>0.1637193340642171</v>
+      </c>
+      <c r="F23" s="14">
         <f>IF(SUM('Balance Sheet'!F4:F5)&gt;0,'Profit &amp; Loss'!F12/SUM('Balance Sheet'!F4:F5),"")</f>
-      </c>
-      <c r="G23" s="14" t="str">
+        <v>0.14782322791095245</v>
+      </c>
+      <c r="G23" s="14">
         <f>IF(SUM('Balance Sheet'!G4:G5)&gt;0,'Profit &amp; Loss'!G12/SUM('Balance Sheet'!G4:G5),"")</f>
-      </c>
-      <c r="H23" s="14" t="str">
+        <v>0.16406097813757628</v>
+      </c>
+      <c r="H23" s="14">
         <f>IF(SUM('Balance Sheet'!H4:H5)&gt;0,'Profit &amp; Loss'!H12/SUM('Balance Sheet'!H4:H5),"")</f>
-      </c>
-      <c r="I23" s="14" t="str">
+        <v>0.11683004680107378</v>
+      </c>
+      <c r="I23" s="14">
         <f>IF(SUM('Balance Sheet'!I4:I5)&gt;0,'Profit &amp; Loss'!I12/SUM('Balance Sheet'!I4:I5),"")</f>
-      </c>
-      <c r="J23" s="14" t="str">
+        <v>0.1169623561805964</v>
+      </c>
+      <c r="J23" s="14">
         <f>IF(SUM('Balance Sheet'!J4:J5)&gt;0,'Profit &amp; Loss'!J12/SUM('Balance Sheet'!J4:J5),"")</f>
-      </c>
-      <c r="K23" s="14" t="str">
+        <v>0.15367393835035045</v>
+      </c>
+      <c r="K23" s="14">
         <f>IF(SUM('Balance Sheet'!K4:K5)&gt;0,'Profit &amp; Loss'!K12/SUM('Balance Sheet'!K4:K5),"")</f>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.1781357487514626</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B24" s="14"/>
-      <c r="C24" s="14" t="str">
+      <c r="C24" s="14">
         <f>IF((B4+B5+B6+C4+C5+C6)&gt;0,('Profit &amp; Loss'!C10+'Profit &amp; Loss'!C9)*2/(B4+B5+B6+C4+C5+C6),"")</f>
-      </c>
-      <c r="D24" s="14" t="str">
+        <v>0.14009265582586272</v>
+      </c>
+      <c r="D24" s="14">
         <f>IF((C4+C5+C6+D4+D5+D6)&gt;0,('Profit &amp; Loss'!D10+'Profit &amp; Loss'!D9)*2/(C4+C5+C6+D4+D5+D6),"")</f>
-      </c>
-      <c r="E24" s="14" t="str">
+        <v>0.16413745134359906</v>
+      </c>
+      <c r="E24" s="14">
         <f>IF((D4+D5+D6+E4+E5+E6)&gt;0,('Profit &amp; Loss'!E10+'Profit &amp; Loss'!E9)*2/(D4+D5+D6+E4+E5+E6),"")</f>
-      </c>
-      <c r="F24" s="14" t="str">
+        <v>0.1365693183027753</v>
+      </c>
+      <c r="F24" s="14">
         <f>IF((E4+E5+E6+F4+F5+F6)&gt;0,('Profit &amp; Loss'!F10+'Profit &amp; Loss'!F9)*2/(E4+E5+E6+F4+F5+F6),"")</f>
-      </c>
-      <c r="G24" s="14" t="str">
+        <v>0.11494487913415771</v>
+      </c>
+      <c r="G24" s="14">
         <f>IF((F4+F5+F6+G4+G5+G6)&gt;0,('Profit &amp; Loss'!G10+'Profit &amp; Loss'!G9)*2/(F4+F5+F6+G4+G5+G6),"")</f>
-      </c>
-      <c r="H24" s="14" t="str">
+        <v>0.14012387584742295</v>
+      </c>
+      <c r="H24" s="14">
         <f>IF((G4+G5+G6+H4+H5+H6)&gt;0,('Profit &amp; Loss'!H10+'Profit &amp; Loss'!H9)*2/(G4+G5+G6+H4+H5+H6),"")</f>
-      </c>
-      <c r="I24" s="14" t="str">
+        <v>0.10587471604289556</v>
+      </c>
+      <c r="I24" s="14">
         <f>IF((H4+H5+H6+I4+I5+I6)&gt;0,('Profit &amp; Loss'!I10+'Profit &amp; Loss'!I9)*2/(H4+H5+H6+I4+I5+I6),"")</f>
-      </c>
-      <c r="J24" s="14" t="str">
+        <v>8.3248784799876768E-2</v>
+      </c>
+      <c r="J24" s="14">
         <f>IF((I4+I5+I6+J4+J5+J6)&gt;0,('Profit &amp; Loss'!J10+'Profit &amp; Loss'!J9)*2/(I4+I5+I6+J4+J5+J6),"")</f>
-      </c>
-      <c r="K24" s="14" t="str">
+        <v>0.12305546732020342</v>
+      </c>
+      <c r="K24" s="14">
         <f>IF((J4+J5+J6+K4+K5+K6)&gt;0,('Profit &amp; Loss'!K10+'Profit &amp; Loss'!K9)*2/(J4+J5+J6+K4+K5+K6),"")</f>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
+        <v>0.14399536370432103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -3706,20 +4200,22 @@
       <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="13.5" style="6" customWidth="1"/>
-    <col min="7" max="11" width="13.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="26.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="13.42578125" style="6" customWidth="1"/>
+    <col min="7" max="11" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="str">
         <f>'Balance Sheet'!A1</f>
+        <v>ADANI PORTS &amp; SPECIAL ECONOMIC ZONE LTD</v>
       </c>
       <c r="E1" t="str">
         <f>UPDATE</f>
+        <v/>
       </c>
       <c r="F1"/>
       <c r="J1" s="4" t="s">
@@ -3727,182 +4223,232 @@
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16">
         <f>'Data Sheet'!B81</f>
+        <v>42460</v>
       </c>
       <c r="C3" s="16">
         <f>'Data Sheet'!C81</f>
+        <v>42825</v>
       </c>
       <c r="D3" s="16">
         <f>'Data Sheet'!D81</f>
+        <v>43190</v>
       </c>
       <c r="E3" s="16">
         <f>'Data Sheet'!E81</f>
+        <v>43555</v>
       </c>
       <c r="F3" s="16">
         <f>'Data Sheet'!F81</f>
+        <v>43921</v>
       </c>
       <c r="G3" s="16">
         <f>'Data Sheet'!G81</f>
+        <v>44286</v>
       </c>
       <c r="H3" s="16">
         <f>'Data Sheet'!H81</f>
+        <v>44651</v>
       </c>
       <c r="I3" s="16">
         <f>'Data Sheet'!I81</f>
+        <v>45016</v>
       </c>
       <c r="J3" s="16">
         <f>'Data Sheet'!J81</f>
+        <v>45382</v>
       </c>
       <c r="K3" s="16">
         <f>'Data Sheet'!K81</f>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="1">
         <f>'Data Sheet'!B82</f>
+        <v>2380.52</v>
       </c>
       <c r="C4" s="1">
         <f>'Data Sheet'!C82</f>
+        <v>4062.57</v>
       </c>
       <c r="D4" s="1">
         <f>'Data Sheet'!D82</f>
+        <v>5608.14</v>
       </c>
       <c r="E4" s="1">
         <f>'Data Sheet'!E82</f>
+        <v>6029.4</v>
       </c>
       <c r="F4" s="1">
         <f>'Data Sheet'!F82</f>
+        <v>7401.81</v>
       </c>
       <c r="G4" s="1">
         <f>'Data Sheet'!G82</f>
+        <v>7555.78</v>
       </c>
       <c r="H4" s="1">
         <f>'Data Sheet'!H82</f>
+        <v>10420.14</v>
       </c>
       <c r="I4" s="1">
         <f>'Data Sheet'!I82</f>
+        <v>11899.5</v>
       </c>
       <c r="J4" s="1">
         <f>'Data Sheet'!J82</f>
+        <v>15017.58</v>
       </c>
       <c r="K4" s="1">
         <f>'Data Sheet'!K82</f>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>17226.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9">
         <f>'Data Sheet'!B83</f>
+        <v>-4153.16</v>
       </c>
       <c r="C5" s="9">
         <f>'Data Sheet'!C83</f>
+        <v>-2629.15</v>
       </c>
       <c r="D5" s="9">
         <f>'Data Sheet'!D83</f>
+        <v>-3845.84</v>
       </c>
       <c r="E5" s="9">
         <f>'Data Sheet'!E83</f>
+        <v>-4368.03</v>
       </c>
       <c r="F5" s="9">
         <f>'Data Sheet'!F83</f>
+        <v>-748.91</v>
       </c>
       <c r="G5" s="9">
         <f>'Data Sheet'!G83</f>
+        <v>-14064.12</v>
       </c>
       <c r="H5" s="9">
         <f>'Data Sheet'!H83</f>
+        <v>-5493.13</v>
       </c>
       <c r="I5" s="9">
         <f>'Data Sheet'!I83</f>
+        <v>-16715.93</v>
       </c>
       <c r="J5" s="9">
         <f>'Data Sheet'!J83</f>
+        <v>-6946.55</v>
       </c>
       <c r="K5" s="9">
         <f>'Data Sheet'!K83</f>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-9787.5300000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="9">
         <f>'Data Sheet'!B84</f>
+        <v>2170.41</v>
       </c>
       <c r="C6" s="9">
         <f>'Data Sheet'!C84</f>
+        <v>-1324.71</v>
       </c>
       <c r="D6" s="9">
         <f>'Data Sheet'!D84</f>
+        <v>-1889.03</v>
       </c>
       <c r="E6" s="9">
         <f>'Data Sheet'!E84</f>
+        <v>2313.34</v>
       </c>
       <c r="F6" s="9">
         <f>'Data Sheet'!F84</f>
+        <v>-4255.63</v>
       </c>
       <c r="G6" s="9">
         <f>'Data Sheet'!G84</f>
+        <v>3513.85</v>
       </c>
       <c r="H6" s="9">
         <f>'Data Sheet'!H84</f>
+        <v>-585.77</v>
       </c>
       <c r="I6" s="9">
         <f>'Data Sheet'!I84</f>
+        <v>-2733.8</v>
       </c>
       <c r="J6" s="9">
         <f>'Data Sheet'!J84</f>
+        <v>-7800.11</v>
       </c>
       <c r="K6" s="9">
         <f>'Data Sheet'!K84</f>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>-6915.52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="1">
         <f>'Data Sheet'!B85</f>
+        <v>397.77</v>
       </c>
       <c r="C7" s="1">
         <f>'Data Sheet'!C85</f>
+        <v>108.71</v>
       </c>
       <c r="D7" s="1">
         <f>'Data Sheet'!D85</f>
+        <v>-126.73</v>
       </c>
       <c r="E7" s="1">
         <f>'Data Sheet'!E85</f>
+        <v>3974.71</v>
       </c>
       <c r="F7" s="1">
         <f>'Data Sheet'!F85</f>
+        <v>2397.27</v>
       </c>
       <c r="G7" s="1">
         <f>'Data Sheet'!G85</f>
+        <v>-2994.49</v>
       </c>
       <c r="H7" s="1">
         <f>'Data Sheet'!H85</f>
+        <v>4341.24</v>
       </c>
       <c r="I7" s="1">
         <f>'Data Sheet'!I85</f>
+        <v>-7550.23</v>
       </c>
       <c r="J7" s="1">
         <f>'Data Sheet'!J85</f>
+        <v>270.92</v>
       </c>
       <c r="K7" s="1">
         <f>'Data Sheet'!K85</f>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>523.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -3915,7 +4461,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="24" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -3935,42 +4481,42 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="8"/>
-    <col min="2" max="2" width="10.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="26" customWidth="1"/>
-    <col min="4" max="5" width="8.83203125" style="11"/>
-    <col min="6" max="6" width="6.83203125" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="8.85546875" style="8"/>
+    <col min="2" max="2" width="10.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="26" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="11"/>
+    <col min="6" max="6" width="6.85546875" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>51</v>
       </c>
@@ -3978,27 +4524,27 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>92</v>
       </c>
@@ -4024,14 +4570,14 @@
       <selection pane="bottomRight" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="13.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="27.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4040,6 +4586,7 @@
       </c>
       <c r="E1" s="32" t="str">
         <f>IF(B2&lt;&gt;B3, "A NEW VERSION OF THE WORKSHEET IS AVAILABLE", "")</f>
+        <v/>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -4048,7 +4595,7 @@
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -4065,7 +4612,7 @@
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -4073,31 +4620,32 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="5">
         <f>IF(B9&gt;0, B9/B8, 0)</f>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>216.01392023237628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B7">
-        <v>2.00</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>43</v>
       </c>
@@ -4105,55 +4653,55 @@
         <v>1342.65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B9">
-        <v>290031.09</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>290031.09000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="16">
-        <v>42460.0</v>
+        <v>42460</v>
       </c>
       <c r="C16" s="16">
-        <v>42825.0</v>
+        <v>42825</v>
       </c>
       <c r="D16" s="16">
-        <v>43190.0</v>
+        <v>43190</v>
       </c>
       <c r="E16" s="16">
-        <v>43555.0</v>
+        <v>43555</v>
       </c>
       <c r="F16" s="16">
-        <v>43921.0</v>
+        <v>43921</v>
       </c>
       <c r="G16" s="16">
-        <v>44286.0</v>
+        <v>44286</v>
       </c>
       <c r="H16" s="16">
-        <v>44651.0</v>
+        <v>44651</v>
       </c>
       <c r="I16" s="16">
-        <v>45016.0</v>
+        <v>45016</v>
       </c>
       <c r="J16" s="16">
-        <v>45382.0</v>
+        <v>45382</v>
       </c>
       <c r="K16" s="16">
-        <v>45747.0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
@@ -4182,13 +4730,13 @@
         <v>20851.91</v>
       </c>
       <c r="J17">
-        <v>26710.56</v>
+        <v>26710.560000000001</v>
       </c>
       <c r="K17">
         <v>30475.33</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -4202,12 +4750,12 @@
         <v>140.43</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -4239,10 +4787,10 @@
         <v>1228.57</v>
       </c>
       <c r="K20">
-        <v>1267.35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1267.3499999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -4268,7 +4816,7 @@
         <v>3950.79</v>
       </c>
       <c r="I21">
-        <v>4742.27</v>
+        <v>4742.2700000000004</v>
       </c>
       <c r="J21">
         <v>6048.03</v>
@@ -4277,7 +4825,7 @@
         <v>7003.68</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -4291,7 +4839,7 @@
         <v>448.15</v>
       </c>
       <c r="E22">
-        <v>530.55</v>
+        <v>530.54999999999995</v>
       </c>
       <c r="F22">
         <v>547.66</v>
@@ -4312,7 +4860,7 @@
         <v>2011.44</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>85</v>
       </c>
@@ -4347,7 +4895,7 @@
         <v>1424.27</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>86</v>
       </c>
@@ -4361,7 +4909,7 @@
         <v>111.88</v>
       </c>
       <c r="E24">
-        <v>591.43</v>
+        <v>591.42999999999995</v>
       </c>
       <c r="F24">
         <v>1796.26</v>
@@ -4370,7 +4918,7 @@
         <v>-558.22</v>
       </c>
       <c r="H24">
-        <v>1057.34</v>
+        <v>1057.3399999999999</v>
       </c>
       <c r="I24">
         <v>2135.9</v>
@@ -4379,10 +4927,10 @@
         <v>525.13</v>
       </c>
       <c r="K24">
-        <v>628.07</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>628.07000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>9</v>
       </c>
@@ -4417,7 +4965,7 @@
         <v>1799.85</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>10</v>
       </c>
@@ -4428,7 +4976,7 @@
         <v>1160.19</v>
       </c>
       <c r="D26">
-        <v>1188.37</v>
+        <v>1188.3699999999999</v>
       </c>
       <c r="E26">
         <v>1373.48</v>
@@ -4452,7 +5000,7 @@
         <v>4378.93</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
@@ -4484,10 +5032,10 @@
         <v>2732.94</v>
       </c>
       <c r="K27">
-        <v>2531.82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2531.8200000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>12</v>
       </c>
@@ -4522,7 +5070,7 @@
         <v>13029.62</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>13</v>
       </c>
@@ -4557,7 +5105,7 @@
         <v>1968.36</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>14</v>
       </c>
@@ -4592,7 +5140,7 @@
         <v>11092.31</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>70</v>
       </c>
@@ -4600,7 +5148,7 @@
         <v>227.8</v>
       </c>
       <c r="C31">
-        <v>269.22</v>
+        <v>269.22000000000003</v>
       </c>
       <c r="D31">
         <v>414.19</v>
@@ -4621,75 +5169,75 @@
         <v>1080.08</v>
       </c>
       <c r="J31">
-        <v>1296.09</v>
+        <v>1296.0899999999999</v>
       </c>
       <c r="K31">
         <v>1512.1</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="16">
-        <v>44926.0</v>
+        <v>44926</v>
       </c>
       <c r="C41" s="16">
-        <v>45016.0</v>
+        <v>45016</v>
       </c>
       <c r="D41" s="16">
-        <v>45107.0</v>
+        <v>45107</v>
       </c>
       <c r="E41" s="16">
-        <v>45199.0</v>
+        <v>45199</v>
       </c>
       <c r="F41" s="16">
-        <v>45291.0</v>
+        <v>45291</v>
       </c>
       <c r="G41" s="16">
-        <v>45382.0</v>
+        <v>45382</v>
       </c>
       <c r="H41" s="16">
-        <v>45473.0</v>
+        <v>45473</v>
       </c>
       <c r="I41" s="16">
-        <v>45565.0</v>
+        <v>45565</v>
       </c>
       <c r="J41" s="16">
-        <v>45657.0</v>
+        <v>45657</v>
       </c>
       <c r="K41" s="16">
-        <v>45747.0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>6</v>
       </c>
@@ -4724,7 +5272,7 @@
         <v>8488.44</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>7</v>
       </c>
@@ -4735,7 +5283,7 @@
         <v>2526.17</v>
       </c>
       <c r="D43">
-        <v>2558.22</v>
+        <v>2558.2199999999998</v>
       </c>
       <c r="E43">
         <v>2982.43</v>
@@ -4759,12 +5307,12 @@
         <v>3482.48</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B44">
-        <v>284.91</v>
+        <v>284.91000000000003</v>
       </c>
       <c r="C44">
         <v>-884.53</v>
@@ -4779,7 +5327,7 @@
         <v>506.85</v>
       </c>
       <c r="G44">
-        <v>-70.26</v>
+        <v>-70.260000000000005</v>
       </c>
       <c r="H44">
         <v>349.16</v>
@@ -4794,7 +5342,7 @@
         <v>425.62</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>10</v>
       </c>
@@ -4829,7 +5377,7 @@
         <v>1184.73</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>11</v>
       </c>
@@ -4837,10 +5385,10 @@
         <v>533.88</v>
       </c>
       <c r="C46">
-        <v>622.56</v>
+        <v>622.55999999999995</v>
       </c>
       <c r="D46">
-        <v>632.69</v>
+        <v>632.69000000000005</v>
       </c>
       <c r="E46">
         <v>520.1</v>
@@ -4864,7 +5412,7 @@
         <v>714.92</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>12</v>
       </c>
@@ -4875,10 +5423,10 @@
         <v>917.23</v>
       </c>
       <c r="D47">
-        <v>2490.74</v>
+        <v>2490.7399999999998</v>
       </c>
       <c r="E47">
-        <v>2520.68</v>
+        <v>2520.6799999999998</v>
       </c>
       <c r="F47">
         <v>2741.33</v>
@@ -4899,7 +5447,7 @@
         <v>3531.93</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>13</v>
       </c>
@@ -4919,7 +5467,7 @@
         <v>533.12</v>
       </c>
       <c r="G48">
-        <v>326.21</v>
+        <v>326.20999999999998</v>
       </c>
       <c r="H48">
         <v>485.42</v>
@@ -4934,7 +5482,7 @@
         <v>508.83</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>14</v>
       </c>
@@ -4945,7 +5493,7 @@
         <v>1157.55</v>
       </c>
       <c r="D49">
-        <v>2114.72</v>
+        <v>2114.7199999999998</v>
       </c>
       <c r="E49">
         <v>1747.85</v>
@@ -4960,16 +5508,16 @@
         <v>3112.83</v>
       </c>
       <c r="I49">
-        <v>2445.0</v>
+        <v>2445</v>
       </c>
       <c r="J49">
-        <v>2520.26</v>
+        <v>2520.2600000000002</v>
       </c>
       <c r="K49">
         <v>3014.22</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>8</v>
       </c>
@@ -4995,68 +5543,68 @@
         <v>4739.42</v>
       </c>
       <c r="I50">
-        <v>4235.27</v>
+        <v>4235.2700000000004</v>
       </c>
       <c r="J50">
-        <v>4802.06</v>
+        <v>4802.0600000000004</v>
       </c>
       <c r="K50">
         <v>5005.96</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B56" s="16">
-        <v>42460.0</v>
+        <v>42460</v>
       </c>
       <c r="C56" s="16">
-        <v>42825.0</v>
+        <v>42825</v>
       </c>
       <c r="D56" s="16">
-        <v>43190.0</v>
+        <v>43190</v>
       </c>
       <c r="E56" s="16">
-        <v>43555.0</v>
+        <v>43555</v>
       </c>
       <c r="F56" s="16">
-        <v>43921.0</v>
+        <v>43921</v>
       </c>
       <c r="G56" s="16">
-        <v>44286.0</v>
+        <v>44286</v>
       </c>
       <c r="H56" s="16">
-        <v>44651.0</v>
+        <v>44651</v>
       </c>
       <c r="I56" s="16">
-        <v>45016.0</v>
+        <v>45016</v>
       </c>
       <c r="J56" s="16">
-        <v>45382.0</v>
+        <v>45382</v>
       </c>
       <c r="K56" s="16">
-        <v>45747.0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>24</v>
       </c>
@@ -5091,7 +5639,7 @@
         <v>432.03</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>25</v>
       </c>
@@ -5102,7 +5650,7 @@
         <v>17111.79</v>
       </c>
       <c r="D58">
-        <v>20488.76</v>
+        <v>20488.759999999998</v>
       </c>
       <c r="E58">
         <v>23958.13</v>
@@ -5126,7 +5674,7 @@
         <v>61836.83</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>71</v>
       </c>
@@ -5155,13 +5703,13 @@
         <v>53434.22</v>
       </c>
       <c r="J59">
-        <v>49470.24</v>
+        <v>49470.239999999998</v>
       </c>
       <c r="K59">
         <v>51620.73</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>72</v>
       </c>
@@ -5181,10 +5729,10 @@
         <v>6217.42</v>
       </c>
       <c r="G60">
-        <v>8284.87</v>
+        <v>8284.8700000000008</v>
       </c>
       <c r="H60">
-        <v>8571.55</v>
+        <v>8571.5499999999993</v>
       </c>
       <c r="I60">
         <v>13739.58</v>
@@ -5193,10 +5741,10 @@
         <v>14750.72</v>
       </c>
       <c r="K60">
-        <v>19553.06</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>19553.060000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>26</v>
       </c>
@@ -5216,7 +5764,7 @@
         <v>61916.7</v>
       </c>
       <c r="G61">
-        <v>74581.93</v>
+        <v>74581.929999999993</v>
       </c>
       <c r="H61">
         <v>98327.99</v>
@@ -5231,7 +5779,7 @@
         <v>133442.65</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>27</v>
       </c>
@@ -5263,10 +5811,10 @@
         <v>75147.81</v>
       </c>
       <c r="K62">
-        <v>89616.32</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+        <v>89616.320000000007</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>28</v>
       </c>
@@ -5280,7 +5828,7 @@
         <v>4545.46</v>
       </c>
       <c r="E63">
-        <v>4483.48</v>
+        <v>4483.4799999999996</v>
       </c>
       <c r="F63">
         <v>3216.33</v>
@@ -5301,15 +5849,15 @@
         <v>11706.1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B64">
-        <v>545.18</v>
+        <v>545.17999999999995</v>
       </c>
       <c r="C64">
-        <v>1161.36</v>
+        <v>1161.3599999999999</v>
       </c>
       <c r="D64">
         <v>1078.92</v>
@@ -5318,7 +5866,7 @@
         <v>782.3</v>
       </c>
       <c r="F64">
-        <v>1178.0</v>
+        <v>1178</v>
       </c>
       <c r="G64">
         <v>2236.15</v>
@@ -5336,7 +5884,7 @@
         <v>4659.45</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>73</v>
       </c>
@@ -5347,7 +5895,7 @@
         <v>16640.54</v>
       </c>
       <c r="D65">
-        <v>18938.33</v>
+        <v>18938.330000000002</v>
       </c>
       <c r="E65">
         <v>22924.23</v>
@@ -5356,22 +5904,22 @@
         <v>24807.86</v>
       </c>
       <c r="G65">
-        <v>20357.69</v>
+        <v>20357.689999999999</v>
       </c>
       <c r="H65">
         <v>28591.43</v>
       </c>
       <c r="I65">
-        <v>26271.04</v>
+        <v>26271.040000000001</v>
       </c>
       <c r="J65">
-        <v>26626.64</v>
+        <v>26626.639999999999</v>
       </c>
       <c r="K65">
         <v>27460.78</v>
       </c>
     </row>
-    <row r="66" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>26</v>
       </c>
@@ -5391,7 +5939,7 @@
         <v>61916.7</v>
       </c>
       <c r="G66">
-        <v>74581.93</v>
+        <v>74581.929999999993</v>
       </c>
       <c r="H66">
         <v>98327.99</v>
@@ -5406,7 +5954,7 @@
         <v>133442.65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>78</v>
       </c>
@@ -5438,10 +5986,10 @@
         <v>3666.94</v>
       </c>
       <c r="K67">
-        <v>4432.36</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+        <v>4432.3599999999997</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>45</v>
       </c>
@@ -5458,7 +6006,7 @@
         <v>806.68</v>
       </c>
       <c r="F68">
-        <v>288.28</v>
+        <v>288.27999999999997</v>
       </c>
       <c r="G68">
         <v>991.85</v>
@@ -5473,10 +6021,10 @@
         <v>437.51</v>
       </c>
       <c r="K68">
-        <v>521.8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+        <v>521.79999999999995</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>87</v>
       </c>
@@ -5502,7 +6050,7 @@
         <v>10667.41</v>
       </c>
       <c r="I69">
-        <v>4334.31</v>
+        <v>4334.3100000000004</v>
       </c>
       <c r="J69">
         <v>7631.88</v>
@@ -5511,140 +6059,140 @@
         <v>6605.97</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B70">
-        <v>2070951761.0</v>
+        <v>2070951761</v>
       </c>
       <c r="C70">
-        <v>2070951761.0</v>
+        <v>2070951761</v>
       </c>
       <c r="D70">
-        <v>2070951761.0</v>
+        <v>2070951761</v>
       </c>
       <c r="E70">
-        <v>2070951761.0</v>
+        <v>2070951761</v>
       </c>
       <c r="F70">
-        <v>2031751761.0</v>
+        <v>2031751761</v>
       </c>
       <c r="G70">
-        <v>2031751761.0</v>
+        <v>2031751761</v>
       </c>
       <c r="H70">
-        <v>2112373230.0</v>
+        <v>2112373230</v>
       </c>
       <c r="I70">
-        <v>2160138945.0</v>
+        <v>2160138945</v>
       </c>
       <c r="J70">
-        <v>2160138945.0</v>
+        <v>2160138945</v>
       </c>
       <c r="K70">
-        <v>2160138945.0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2160138945</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="J72">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K72">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="9"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="9"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="9"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="9"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B81" s="16">
-        <v>42460.0</v>
+        <v>42460</v>
       </c>
       <c r="C81" s="16">
-        <v>42825.0</v>
+        <v>42825</v>
       </c>
       <c r="D81" s="16">
-        <v>43190.0</v>
+        <v>43190</v>
       </c>
       <c r="E81" s="16">
-        <v>43555.0</v>
+        <v>43555</v>
       </c>
       <c r="F81" s="16">
-        <v>43921.0</v>
+        <v>43921</v>
       </c>
       <c r="G81" s="16">
-        <v>44286.0</v>
+        <v>44286</v>
       </c>
       <c r="H81" s="16">
-        <v>44651.0</v>
+        <v>44651</v>
       </c>
       <c r="I81" s="16">
-        <v>45016.0</v>
+        <v>45016</v>
       </c>
       <c r="J81" s="16">
-        <v>45382.0</v>
+        <v>45382</v>
       </c>
       <c r="K81" s="16">
-        <v>45747.0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>32</v>
       </c>
@@ -5679,7 +6227,7 @@
         <v>17226.28</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>33</v>
       </c>
@@ -5711,10 +6259,10 @@
         <v>-6946.55</v>
       </c>
       <c r="K83">
-        <v>-9787.53</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>-9787.5300000000007</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>34</v>
       </c>
@@ -5749,7 +6297,7 @@
         <v>-6915.52</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>35</v>
       </c>
@@ -5784,19 +6332,19 @@
         <v>523.23</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="9"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="9"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="9"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="9"/>
     </row>
-    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>77</v>
       </c>
@@ -5831,12 +6379,12 @@
         <v>1182.95</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
add and modified excel files
</commit_message>
<xml_diff>
--- a/data/downloads/Adani Ports.xlsx
+++ b/data/downloads/Adani Ports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\finance_project\data\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratyush/Websites/screener/company/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84EAF486-6F84-4425-8E5E-118381173088}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AC4F62-F3F6-2E4B-8F69-3E72AC5D7A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profit &amp; Loss" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,13 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -335,8 +342,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
@@ -457,7 +464,7 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -469,19 +476,19 @@
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -491,13 +498,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -511,11 +518,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -526,7 +533,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="6" builtinId="5"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
@@ -1717,28 +1724,26 @@
       <selection activeCell="I2" sqref="I2"/>
       <selection pane="topRight" activeCell="I2" sqref="I2"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="6" customWidth="1"/>
-    <col min="2" max="6" width="13.42578125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.42578125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="6" customWidth="1"/>
-    <col min="13" max="14" width="12.140625" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="20.6640625" style="6" customWidth="1"/>
+    <col min="2" max="6" width="13.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.5" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="6" customWidth="1"/>
+    <col min="13" max="14" width="12.1640625" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="str">
         <f>'Data Sheet'!B1</f>
-        <v>ADANI PORTS &amp; SPECIAL ECONOMIC ZONE LTD</v>
       </c>
       <c r="H1" t="str">
         <f>UPDATE</f>
-        <v/>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -1746,49 +1751,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16">
         <f>'Data Sheet'!B16</f>
-        <v>42460</v>
       </c>
       <c r="C3" s="16">
         <f>'Data Sheet'!C16</f>
-        <v>42825</v>
       </c>
       <c r="D3" s="16">
         <f>'Data Sheet'!D16</f>
-        <v>43190</v>
       </c>
       <c r="E3" s="16">
         <f>'Data Sheet'!E16</f>
-        <v>43555</v>
       </c>
       <c r="F3" s="16">
         <f>'Data Sheet'!F16</f>
-        <v>43921</v>
       </c>
       <c r="G3" s="16">
         <f>'Data Sheet'!G16</f>
-        <v>44286</v>
       </c>
       <c r="H3" s="16">
         <f>'Data Sheet'!H16</f>
-        <v>44651</v>
       </c>
       <c r="I3" s="16">
         <f>'Data Sheet'!I16</f>
-        <v>45016</v>
       </c>
       <c r="J3" s="16">
         <f>'Data Sheet'!J16</f>
-        <v>45382</v>
       </c>
       <c r="K3" s="16">
         <f>'Data Sheet'!K16</f>
-        <v>45747</v>
       </c>
       <c r="L3" s="17" t="s">
         <v>3</v>
@@ -1800,224 +1795,174 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
         <f>'Data Sheet'!B17</f>
-        <v>7108.65</v>
       </c>
       <c r="C4" s="1">
         <f>'Data Sheet'!C17</f>
-        <v>8439.35</v>
       </c>
       <c r="D4" s="1">
         <f>'Data Sheet'!D17</f>
-        <v>11322.96</v>
       </c>
       <c r="E4" s="1">
         <f>'Data Sheet'!E17</f>
-        <v>10925.44</v>
       </c>
       <c r="F4" s="1">
         <f>'Data Sheet'!F17</f>
-        <v>11873.07</v>
       </c>
       <c r="G4" s="1">
         <f>'Data Sheet'!G17</f>
-        <v>12549.6</v>
       </c>
       <c r="H4" s="1">
         <f>'Data Sheet'!H17</f>
-        <v>17118.79</v>
       </c>
       <c r="I4" s="1">
         <f>'Data Sheet'!I17</f>
-        <v>20851.91</v>
       </c>
       <c r="J4" s="1">
         <f>'Data Sheet'!J17</f>
-        <v>26710.560000000001</v>
       </c>
       <c r="K4" s="1">
         <f>'Data Sheet'!K17</f>
-        <v>30475.33</v>
       </c>
       <c r="L4" s="1">
         <f>SUM(Quarters!H4:K4)</f>
-        <v>31078.6</v>
       </c>
       <c r="M4" s="1">
         <f>$K4+M23*K4</f>
-        <v>36935.178419121592</v>
       </c>
       <c r="N4" s="1">
         <f>$K4+N23*L4</f>
-        <v>34855.761594170996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="9">
         <f>SUM('Data Sheet'!B18,'Data Sheet'!B20:B24, -1*'Data Sheet'!B19)</f>
-        <v>2531.7000000000003</v>
       </c>
       <c r="C5" s="9">
         <f>SUM('Data Sheet'!C18,'Data Sheet'!C20:C24, -1*'Data Sheet'!C19)</f>
-        <v>3021.12</v>
       </c>
       <c r="D5" s="9">
         <f>SUM('Data Sheet'!D18,'Data Sheet'!D20:D24, -1*'Data Sheet'!D19)</f>
-        <v>4166.29</v>
       </c>
       <c r="E5" s="9">
         <f>SUM('Data Sheet'!E18,'Data Sheet'!E20:E24, -1*'Data Sheet'!E19)</f>
-        <v>4329.8</v>
       </c>
       <c r="F5" s="9">
         <f>SUM('Data Sheet'!F18,'Data Sheet'!F20:F24, -1*'Data Sheet'!F19)</f>
-        <v>5925.96</v>
       </c>
       <c r="G5" s="9">
         <f>SUM('Data Sheet'!G18,'Data Sheet'!G20:G24, -1*'Data Sheet'!G19)</f>
-        <v>3861.6399999999994</v>
       </c>
       <c r="H5" s="9">
         <f>SUM('Data Sheet'!H18,'Data Sheet'!H20:H24, -1*'Data Sheet'!H19)</f>
-        <v>7590.83</v>
       </c>
       <c r="I5" s="9">
         <f>SUM('Data Sheet'!I18,'Data Sheet'!I20:I24, -1*'Data Sheet'!I19)</f>
-        <v>9904.7800000000007</v>
       </c>
       <c r="J5" s="9">
         <f>SUM('Data Sheet'!J18,'Data Sheet'!J20:J24, -1*'Data Sheet'!J19)</f>
-        <v>11121.149999999998</v>
       </c>
       <c r="K5" s="9">
         <f>SUM('Data Sheet'!K18,'Data Sheet'!K20:K24, -1*'Data Sheet'!K19)</f>
-        <v>12334.810000000001</v>
       </c>
       <c r="L5" s="9">
         <f>SUM(Quarters!H5:K5)</f>
-        <v>12295.89</v>
       </c>
       <c r="M5" s="9">
         <f t="shared" ref="M5:N5" si="0">M4-M6</f>
-        <v>14612.977771582147</v>
       </c>
       <c r="N5" s="9">
         <f t="shared" si="0"/>
-        <v>14900.650710875037</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
         <f>B4-B5</f>
-        <v>4576.9499999999989</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ref="C6:K6" si="1">C4-C5</f>
-        <v>5418.2300000000005</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>7156.6699999999992</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>6595.64</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>5947.11</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>8687.9600000000009</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>9527.9600000000009</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>10947.13</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
-        <v>15589.410000000003</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="1"/>
-        <v>18140.52</v>
       </c>
       <c r="L6" s="1">
         <f>SUM(Quarters!H6:K6)</f>
-        <v>18782.71</v>
       </c>
       <c r="M6" s="1">
         <f>M4*M24</f>
-        <v>22322.200647539445</v>
       </c>
       <c r="N6" s="1">
         <f>N4*N24</f>
-        <v>19955.110883295958</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="9">
         <f>'Data Sheet'!B25</f>
-        <v>729.75</v>
       </c>
       <c r="C7" s="9">
         <f>'Data Sheet'!C25</f>
-        <v>1036.57</v>
       </c>
       <c r="D7" s="9">
         <f>'Data Sheet'!D25</f>
-        <v>844.49</v>
       </c>
       <c r="E7" s="9">
         <f>'Data Sheet'!E25</f>
-        <v>1289.25</v>
       </c>
       <c r="F7" s="9">
         <f>'Data Sheet'!F25</f>
-        <v>1927.73</v>
       </c>
       <c r="G7" s="9">
         <f>'Data Sheet'!G25</f>
-        <v>1966.68</v>
       </c>
       <c r="H7" s="9">
         <f>'Data Sheet'!H25</f>
-        <v>1832.4</v>
       </c>
       <c r="I7" s="9">
         <f>'Data Sheet'!I25</f>
-        <v>327.11</v>
       </c>
       <c r="J7" s="9">
         <f>'Data Sheet'!J25</f>
-        <v>670.56</v>
       </c>
       <c r="K7" s="9">
         <f>'Data Sheet'!K25</f>
-        <v>1799.85</v>
       </c>
       <c r="L7" s="9">
         <f>SUM(Quarters!H7:K7)</f>
-        <v>1275.21</v>
       </c>
       <c r="M7" s="9">
         <v>0</v>
@@ -2026,562 +1971,437 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="9">
         <f>'Data Sheet'!B26</f>
-        <v>1062.96</v>
       </c>
       <c r="C8" s="9">
         <f>'Data Sheet'!C26</f>
-        <v>1160.19</v>
       </c>
       <c r="D8" s="9">
         <f>'Data Sheet'!D26</f>
-        <v>1188.3699999999999</v>
       </c>
       <c r="E8" s="9">
         <f>'Data Sheet'!E26</f>
-        <v>1373.48</v>
       </c>
       <c r="F8" s="9">
         <f>'Data Sheet'!F26</f>
-        <v>1680.28</v>
       </c>
       <c r="G8" s="9">
         <f>'Data Sheet'!G26</f>
-        <v>2107.34</v>
       </c>
       <c r="H8" s="9">
         <f>'Data Sheet'!H26</f>
-        <v>3099.3</v>
       </c>
       <c r="I8" s="9">
         <f>'Data Sheet'!I26</f>
-        <v>3424.71</v>
       </c>
       <c r="J8" s="9">
         <f>'Data Sheet'!J26</f>
-        <v>3888.46</v>
       </c>
       <c r="K8" s="9">
         <f>'Data Sheet'!K26</f>
-        <v>4378.93</v>
       </c>
       <c r="L8" s="9">
         <f>SUM(Quarters!H8:K8)</f>
-        <v>4378.93</v>
       </c>
       <c r="M8" s="9">
         <f>+$L8</f>
-        <v>4378.93</v>
       </c>
       <c r="N8" s="9">
         <f>+$L8</f>
-        <v>4378.93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9">
         <f>'Data Sheet'!B27</f>
-        <v>1124.3</v>
       </c>
       <c r="C9" s="9">
         <f>'Data Sheet'!C27</f>
-        <v>1115.74</v>
       </c>
       <c r="D9" s="9">
         <f>'Data Sheet'!D27</f>
-        <v>1578.66</v>
       </c>
       <c r="E9" s="9">
         <f>'Data Sheet'!E27</f>
-        <v>1385.19</v>
       </c>
       <c r="F9" s="9">
         <f>'Data Sheet'!F27</f>
-        <v>1950.64</v>
       </c>
       <c r="G9" s="9">
         <f>'Data Sheet'!G27</f>
-        <v>2255.29</v>
       </c>
       <c r="H9" s="9">
         <f>'Data Sheet'!H27</f>
-        <v>2543.92</v>
       </c>
       <c r="I9" s="9">
         <f>'Data Sheet'!I27</f>
-        <v>2362.64</v>
       </c>
       <c r="J9" s="9">
         <f>'Data Sheet'!J27</f>
-        <v>2732.94</v>
       </c>
       <c r="K9" s="9">
         <f>'Data Sheet'!K27</f>
-        <v>2531.8200000000002</v>
       </c>
       <c r="L9" s="9">
         <f>SUM(Quarters!H9:K9)</f>
-        <v>2649.37</v>
       </c>
       <c r="M9" s="9">
         <f>+$L9</f>
-        <v>2649.37</v>
       </c>
       <c r="N9" s="9">
         <f>+$L9</f>
-        <v>2649.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="9">
         <f>'Data Sheet'!B28</f>
-        <v>3119.44</v>
       </c>
       <c r="C10" s="9">
         <f>'Data Sheet'!C28</f>
-        <v>4178.87</v>
       </c>
       <c r="D10" s="9">
         <f>'Data Sheet'!D28</f>
-        <v>5234.13</v>
       </c>
       <c r="E10" s="9">
         <f>'Data Sheet'!E28</f>
-        <v>5126.22</v>
       </c>
       <c r="F10" s="9">
         <f>'Data Sheet'!F28</f>
-        <v>4243.92</v>
       </c>
       <c r="G10" s="9">
         <f>'Data Sheet'!G28</f>
-        <v>6292.01</v>
       </c>
       <c r="H10" s="9">
         <f>'Data Sheet'!H28</f>
-        <v>5717.14</v>
       </c>
       <c r="I10" s="9">
         <f>'Data Sheet'!I28</f>
-        <v>5486.89</v>
       </c>
       <c r="J10" s="9">
         <f>'Data Sheet'!J28</f>
-        <v>9638.57</v>
       </c>
       <c r="K10" s="9">
         <f>'Data Sheet'!K28</f>
-        <v>13029.62</v>
       </c>
       <c r="L10" s="9">
         <f>SUM(Quarters!H10:K10)</f>
-        <v>13029.619999999999</v>
       </c>
       <c r="M10" s="9">
         <f>M6+M7-SUM(M8:M9)</f>
-        <v>15293.900647539445</v>
       </c>
       <c r="N10" s="9">
         <f>N6+N7-SUM(N8:N9)</f>
-        <v>12926.810883295959</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="9">
         <f>'Data Sheet'!B29</f>
-        <v>282.81</v>
       </c>
       <c r="C11" s="9">
         <f>'Data Sheet'!C29</f>
-        <v>286.63</v>
       </c>
       <c r="D11" s="9">
         <f>'Data Sheet'!D29</f>
-        <v>1544.18</v>
       </c>
       <c r="E11" s="9">
         <f>'Data Sheet'!E29</f>
-        <v>1081.47</v>
       </c>
       <c r="F11" s="9">
         <f>'Data Sheet'!F29</f>
-        <v>459.39</v>
       </c>
       <c r="G11" s="9">
         <f>'Data Sheet'!G29</f>
-        <v>1243.27</v>
       </c>
       <c r="H11" s="9">
         <f>'Data Sheet'!H29</f>
-        <v>763.96</v>
       </c>
       <c r="I11" s="9">
         <f>'Data Sheet'!I29</f>
-        <v>96.04</v>
       </c>
       <c r="J11" s="9">
         <f>'Data Sheet'!J29</f>
-        <v>1534.58</v>
       </c>
       <c r="K11" s="9">
         <f>'Data Sheet'!K29</f>
-        <v>1968.36</v>
       </c>
       <c r="L11" s="9">
         <f>SUM(Quarters!H11:K11)</f>
-        <v>1968.36</v>
       </c>
       <c r="M11" s="10">
         <f>IF($L10&gt;0,$L11/$L10,0)</f>
-        <v>0.1510681048257739</v>
       </c>
       <c r="N11" s="10">
         <f>IF($L10&gt;0,$L11/$L10,0)</f>
-        <v>0.1510681048257739</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1">
         <f>'Data Sheet'!B30</f>
-        <v>2897.16</v>
       </c>
       <c r="C12" s="1">
         <f>'Data Sheet'!C30</f>
-        <v>3911.52</v>
       </c>
       <c r="D12" s="1">
         <f>'Data Sheet'!D30</f>
-        <v>3673.62</v>
       </c>
       <c r="E12" s="1">
         <f>'Data Sheet'!E30</f>
-        <v>3990.22</v>
       </c>
       <c r="F12" s="1">
         <f>'Data Sheet'!F30</f>
-        <v>3763.13</v>
       </c>
       <c r="G12" s="1">
         <f>'Data Sheet'!G30</f>
-        <v>4994.3</v>
       </c>
       <c r="H12" s="1">
         <f>'Data Sheet'!H30</f>
-        <v>4886.03</v>
       </c>
       <c r="I12" s="1">
         <f>'Data Sheet'!I30</f>
-        <v>5308.85</v>
       </c>
       <c r="J12" s="1">
         <f>'Data Sheet'!J30</f>
-        <v>8110.64</v>
       </c>
       <c r="K12" s="1">
         <f>'Data Sheet'!K30</f>
-        <v>11092.31</v>
       </c>
       <c r="L12" s="1">
         <f>SUM(Quarters!H12:K12)</f>
-        <v>11092.31</v>
       </c>
       <c r="M12" s="1">
         <f>M10-M11*M10</f>
-        <v>12983.480061321985</v>
       </c>
       <c r="N12" s="1">
         <f>N10-N11*N10</f>
-        <v>10973.982061715251</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="9">
         <f>IF('Data Sheet'!B93&gt;0,B12/'Data Sheet'!B93,0)</f>
-        <v>13.989183969097054</v>
       </c>
       <c r="C13" s="9">
         <f>IF('Data Sheet'!C93&gt;0,C12/'Data Sheet'!C93,0)</f>
-        <v>18.887107677450508</v>
       </c>
       <c r="D13" s="9">
         <f>IF('Data Sheet'!D93&gt;0,D12/'Data Sheet'!D93,0)</f>
-        <v>17.738387252535006</v>
       </c>
       <c r="E13" s="9">
         <f>IF('Data Sheet'!E93&gt;0,E12/'Data Sheet'!E93,0)</f>
-        <v>19.267117334620956</v>
       </c>
       <c r="F13" s="9">
         <f>IF('Data Sheet'!F93&gt;0,F12/'Data Sheet'!F93,0)</f>
-        <v>18.521163500344521</v>
       </c>
       <c r="G13" s="9">
         <f>IF('Data Sheet'!G93&gt;0,G12/'Data Sheet'!G93,0)</f>
-        <v>24.580667388522492</v>
       </c>
       <c r="H13" s="9">
         <f>IF('Data Sheet'!H93&gt;0,H12/'Data Sheet'!H93,0)</f>
-        <v>23.130231016852868</v>
       </c>
       <c r="I13" s="9">
         <f>IF('Data Sheet'!I93&gt;0,I12/'Data Sheet'!I93,0)</f>
-        <v>24.576871441136987</v>
       </c>
       <c r="J13" s="9">
         <f>IF('Data Sheet'!J93&gt;0,J12/'Data Sheet'!J93,0)</f>
-        <v>37.547520948104257</v>
       </c>
       <c r="K13" s="9">
         <f>IF('Data Sheet'!K93&gt;0,K12/'Data Sheet'!K93,0)</f>
-        <v>51.350909680107399</v>
       </c>
       <c r="L13" s="9">
         <f>IF('Data Sheet'!$B6&gt;0,'Profit &amp; Loss'!L12/'Data Sheet'!$B6,0)</f>
-        <v>51.349977761004858</v>
       </c>
       <c r="M13" s="9">
         <f>IF('Data Sheet'!$B6&gt;0,'Profit &amp; Loss'!M12/'Data Sheet'!$B6,0)</f>
-        <v>60.104830500530007</v>
       </c>
       <c r="N13" s="9">
         <f>IF('Data Sheet'!$B6&gt;0,'Profit &amp; Loss'!N12/'Data Sheet'!$B6,0)</f>
-        <v>50.802198533826086</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="9" t="str">
         <f>IF(B15&gt;0,B15/B13,"")</f>
-        <v>17.70653674633089</v>
-      </c>
-      <c r="C14" s="9">
+      </c>
+      <c r="C14" s="9" t="str">
         <f t="shared" ref="C14:K14" si="2">IF(C15&gt;0,C15/C13,"")</f>
-        <v>17.980519082095963</v>
-      </c>
-      <c r="D14" s="9">
+      </c>
+      <c r="D14" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>19.962355932295669</v>
-      </c>
-      <c r="E14" s="9">
+      </c>
+      <c r="E14" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>19.626703540155681</v>
-      </c>
-      <c r="F14" s="9">
+      </c>
+      <c r="F14" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>13.568262058446029</v>
-      </c>
-      <c r="G14" s="9">
+      </c>
+      <c r="G14" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>28.575302244558795</v>
-      </c>
-      <c r="H14" s="9">
+      </c>
+      <c r="H14" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>33.47134749479639</v>
-      </c>
-      <c r="I14" s="9">
+      </c>
+      <c r="I14" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>25.711165129924556</v>
-      </c>
-      <c r="J14" s="9">
+      </c>
+      <c r="J14" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>35.737379356006429</v>
-      </c>
-      <c r="K14" s="9">
+      </c>
+      <c r="K14" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>23.036592873801762</v>
       </c>
       <c r="L14" s="9">
         <f t="shared" ref="L14" si="3">IF(L13&gt;0,L15/L13,0)</f>
-        <v>26.147041508937278</v>
       </c>
       <c r="M14" s="9">
         <f>M25</f>
-        <v>27.658044717167506</v>
       </c>
       <c r="N14" s="9">
         <f>N25</f>
-        <v>23.774836906122676</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="1">
         <f>'Data Sheet'!B90</f>
-        <v>247.7</v>
       </c>
       <c r="C15" s="1">
         <f>'Data Sheet'!C90</f>
-        <v>339.6</v>
       </c>
       <c r="D15" s="1">
         <f>'Data Sheet'!D90</f>
-        <v>354.1</v>
       </c>
       <c r="E15" s="1">
         <f>'Data Sheet'!E90</f>
-        <v>378.15</v>
       </c>
       <c r="F15" s="1">
         <f>'Data Sheet'!F90</f>
-        <v>251.3</v>
       </c>
       <c r="G15" s="1">
         <f>'Data Sheet'!G90</f>
-        <v>702.4</v>
       </c>
       <c r="H15" s="1">
         <f>'Data Sheet'!H90</f>
-        <v>774.2</v>
       </c>
       <c r="I15" s="1">
         <f>'Data Sheet'!I90</f>
-        <v>631.9</v>
       </c>
       <c r="J15" s="1">
         <f>'Data Sheet'!J90</f>
-        <v>1341.85</v>
       </c>
       <c r="K15" s="1">
         <f>'Data Sheet'!K90</f>
-        <v>1182.95</v>
       </c>
       <c r="L15" s="1">
         <f>'Data Sheet'!B8</f>
-        <v>1342.65</v>
       </c>
       <c r="M15" s="12">
         <f>M13*M14</f>
-        <v>1662.3820897014323</v>
       </c>
       <c r="N15" s="13">
         <f>N13*N14</f>
-        <v>1207.8139846141798</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="7">
         <f>IF('Data Sheet'!B30&gt;0, 'Data Sheet'!B31/'Data Sheet'!B30, 0)</f>
-        <v>7.8628726062764928E-2</v>
       </c>
       <c r="C18" s="7">
         <f>IF('Data Sheet'!C30&gt;0, 'Data Sheet'!C31/'Data Sheet'!C30, 0)</f>
-        <v>6.882746349245307E-2</v>
       </c>
       <c r="D18" s="7">
         <f>IF('Data Sheet'!D30&gt;0, 'Data Sheet'!D31/'Data Sheet'!D30, 0)</f>
-        <v>0.11274709959113899</v>
       </c>
       <c r="E18" s="7">
         <f>IF('Data Sheet'!E30&gt;0, 'Data Sheet'!E31/'Data Sheet'!E30, 0)</f>
-        <v>1.0380380029171325E-2</v>
       </c>
       <c r="F18" s="7">
         <f>IF('Data Sheet'!F30&gt;0, 'Data Sheet'!F31/'Data Sheet'!F30, 0)</f>
-        <v>0.17277107089045554</v>
       </c>
       <c r="G18" s="7">
         <f>IF('Data Sheet'!G30&gt;0, 'Data Sheet'!G31/'Data Sheet'!G30, 0)</f>
-        <v>0.20340788498888732</v>
       </c>
       <c r="H18" s="7">
         <f>IF('Data Sheet'!H30&gt;0, 'Data Sheet'!H31/'Data Sheet'!H30, 0)</f>
-        <v>0.21616322454016862</v>
       </c>
       <c r="I18" s="7">
         <f>IF('Data Sheet'!I30&gt;0, 'Data Sheet'!I31/'Data Sheet'!I30, 0)</f>
-        <v>0.20344895787223219</v>
       </c>
       <c r="J18" s="7">
         <f>IF('Data Sheet'!J30&gt;0, 'Data Sheet'!J31/'Data Sheet'!J30, 0)</f>
-        <v>0.15980119941213022</v>
       </c>
       <c r="K18" s="7">
         <f>IF('Data Sheet'!K30&gt;0, 'Data Sheet'!K31/'Data Sheet'!K30, 0)</f>
-        <v>0.13631966650769767</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="7">
         <f t="shared" ref="B19:L19" si="4">IF(B6&gt;0,B6/B4,0)</f>
-        <v>0.64385642843577884</v>
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:K19" si="5">IF(C6&gt;0,C6/C4,0)</f>
-        <v>0.64201982380159617</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="5"/>
-        <v>0.63204939344482358</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="5"/>
-        <v>0.60369559486849045</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="5"/>
-        <v>0.50089067107327756</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="5"/>
-        <v>0.69228979409702307</v>
       </c>
       <c r="H19" s="7">
         <f t="shared" si="5"/>
-        <v>0.55657905728150181</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" si="5"/>
-        <v>0.52499411324909806</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="5"/>
-        <v>0.58364219993890065</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="5"/>
-        <v>0.59525261908566696</v>
       </c>
       <c r="L19" s="7">
         <f t="shared" si="4"/>
-        <v>0.60436152207628402</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -2594,7 +2414,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -2607,7 +2427,7 @@
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
     </row>
-    <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -2639,7 +2459,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -2649,99 +2469,78 @@
       <c r="G23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="7" t="str">
         <f>IF(B4=0,"",POWER($K4/B4,1/9)-1)</f>
-        <v>0.17554739326307089</v>
-      </c>
-      <c r="I23" s="7">
+      </c>
+      <c r="I23" s="7" t="str">
         <f>IF(D4=0,"",POWER($K4/D4,1/7)-1)</f>
-        <v>0.15193220601280966</v>
-      </c>
-      <c r="J23" s="7">
+      </c>
+      <c r="J23" s="7" t="str">
         <f>IF(F4=0,"",POWER($K4/F4,1/5)-1)</f>
-        <v>0.20747202514220509</v>
-      </c>
-      <c r="K23" s="7">
+      </c>
+      <c r="K23" s="7" t="str">
         <f>IF(H4=0,"",POWER($K4/H4, 1/3)-1)</f>
-        <v>0.2119697610861504</v>
-      </c>
-      <c r="L23" s="7">
+      </c>
+      <c r="L23" s="7" t="str">
         <f>IF(ISERROR(MAX(IF(J4=0,"",(K4-J4)/J4),IF(K4=0,"",(L4-K4)/K4))),"",MAX(IF(J4=0,"",(K4-J4)/J4),IF(K4=0,"",(L4-K4)/K4)))</f>
-        <v>0.14094687644137749</v>
       </c>
       <c r="M23" s="22">
         <f>MAX(K23:L23)</f>
-        <v>0.2119697610861504</v>
       </c>
       <c r="N23" s="22">
         <f>MIN(H23:L23)</f>
-        <v>0.14094687644137749</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="7" t="str">
         <f>IF(SUM(B4:$K$4)=0,"",SUMPRODUCT(B19:$K$19,B4:$K$4)/SUM(B4:$K$4))</f>
-        <v>0.58832210775160532</v>
-      </c>
-      <c r="I24" s="7">
+      </c>
+      <c r="I24" s="7" t="str">
         <f>IF(SUM(E4:$K$4)=0,"",SUMPRODUCT(E19:$K$19,E4:$K$4)/SUM(E4:$K$4))</f>
-        <v>0.57803075291541228</v>
-      </c>
-      <c r="J24" s="7">
+      </c>
+      <c r="J24" s="7" t="str">
         <f>IF(SUM(G4:$K$4)=0,"",SUMPRODUCT(G19:$K$19,G4:$K$4)/SUM(G4:$K$4))</f>
-        <v>0.58393096998417648</v>
-      </c>
-      <c r="K24" s="7">
+      </c>
+      <c r="K24" s="7" t="str">
         <f>IF(SUM(I4:$K$4)=0, "", SUMPRODUCT(I19:$K$19,I4:$K$4)/SUM(I4:$K$4))</f>
-        <v>0.57250537560002979</v>
       </c>
       <c r="L24" s="7">
         <f>L19</f>
-        <v>0.60436152207628402</v>
       </c>
       <c r="M24" s="22">
         <f>MAX(K24:L24)</f>
-        <v>0.60436152207628402</v>
       </c>
       <c r="N24" s="22">
         <f>MIN(H24:L24)</f>
-        <v>0.57250537560002979</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="9" t="str">
         <f>IF(ISERROR(AVERAGEIF(B14:$L14,"&gt;0")),"",AVERAGEIF(B14:$L14,"&gt;0"))</f>
-        <v>23.774836906122676</v>
-      </c>
-      <c r="I25" s="9">
+      </c>
+      <c r="I25" s="9" t="str">
         <f>IF(ISERROR(AVERAGEIF(E14:$L14,"&gt;0")),"",AVERAGEIF(E14:$L14,"&gt;0"))</f>
-        <v>25.734224275828367</v>
-      </c>
-      <c r="J25" s="9">
+      </c>
+      <c r="J25" s="9" t="str">
         <f>IF(ISERROR(AVERAGEIF(G14:$L14,"&gt;0")),"",AVERAGEIF(G14:$L14,"&gt;0"))</f>
-        <v>28.779804768004198</v>
-      </c>
-      <c r="K25" s="9">
+      </c>
+      <c r="K25" s="9" t="str">
         <f>IF(ISERROR(AVERAGEIF(I14:$L14,"&gt;0")),"",AVERAGEIF(I14:$L14,"&gt;0"))</f>
-        <v>27.658044717167506</v>
       </c>
       <c r="L25" s="9">
         <f>L14</f>
-        <v>26.147041508937278</v>
       </c>
       <c r="M25" s="1">
         <f>MAX(K25:L25)</f>
-        <v>27.658044717167506</v>
       </c>
       <c r="N25" s="1">
         <f>MIN(H25:L25)</f>
-        <v>23.774836906122676</v>
       </c>
     </row>
   </sheetData>
@@ -2771,523 +2570,411 @@
       <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="6" customWidth="1"/>
-    <col min="2" max="11" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="20.6640625" style="6" customWidth="1"/>
+    <col min="2" max="11" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="str">
         <f>'Profit &amp; Loss'!A1</f>
-        <v>ADANI PORTS &amp; SPECIAL ECONOMIC ZONE LTD</v>
       </c>
       <c r="E1" t="str">
         <f>UPDATE</f>
-        <v/>
       </c>
       <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16">
         <f>'Data Sheet'!B41</f>
-        <v>44926</v>
       </c>
       <c r="C3" s="16">
         <f>'Data Sheet'!C41</f>
-        <v>45016</v>
       </c>
       <c r="D3" s="16">
         <f>'Data Sheet'!D41</f>
-        <v>45107</v>
       </c>
       <c r="E3" s="16">
         <f>'Data Sheet'!E41</f>
-        <v>45199</v>
       </c>
       <c r="F3" s="16">
         <f>'Data Sheet'!F41</f>
-        <v>45291</v>
       </c>
       <c r="G3" s="16">
         <f>'Data Sheet'!G41</f>
-        <v>45382</v>
       </c>
       <c r="H3" s="16">
         <f>'Data Sheet'!H41</f>
-        <v>45473</v>
       </c>
       <c r="I3" s="16">
         <f>'Data Sheet'!I41</f>
-        <v>45565</v>
       </c>
       <c r="J3" s="16">
         <f>'Data Sheet'!J41</f>
-        <v>45657</v>
       </c>
       <c r="K3" s="16">
         <f>'Data Sheet'!K41</f>
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
         <f>'Data Sheet'!B42</f>
-        <v>4786.17</v>
       </c>
       <c r="C4" s="1">
         <f>'Data Sheet'!C42</f>
-        <v>5796.85</v>
       </c>
       <c r="D4" s="1">
         <f>'Data Sheet'!D42</f>
-        <v>6247.55</v>
       </c>
       <c r="E4" s="1">
         <f>'Data Sheet'!E42</f>
-        <v>6646.41</v>
       </c>
       <c r="F4" s="1">
         <f>'Data Sheet'!F42</f>
-        <v>6920.1</v>
       </c>
       <c r="G4" s="1">
         <f>'Data Sheet'!G42</f>
-        <v>6896.5</v>
       </c>
       <c r="H4" s="1">
         <f>'Data Sheet'!H42</f>
-        <v>7559.59</v>
       </c>
       <c r="I4" s="1">
         <f>'Data Sheet'!I42</f>
-        <v>7067.02</v>
       </c>
       <c r="J4" s="1">
         <f>'Data Sheet'!J42</f>
-        <v>7963.55</v>
       </c>
       <c r="K4" s="1">
         <f>'Data Sheet'!K42</f>
-        <v>8488.44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="9">
         <f>'Data Sheet'!B43</f>
-        <v>2089.67</v>
       </c>
       <c r="C5" s="9">
         <f>'Data Sheet'!C43</f>
-        <v>2526.17</v>
       </c>
       <c r="D5" s="9">
         <f>'Data Sheet'!D43</f>
-        <v>2558.2199999999998</v>
       </c>
       <c r="E5" s="9">
         <f>'Data Sheet'!E43</f>
-        <v>2982.43</v>
       </c>
       <c r="F5" s="9">
         <f>'Data Sheet'!F43</f>
-        <v>2724.42</v>
       </c>
       <c r="G5" s="9">
         <f>'Data Sheet'!G43</f>
-        <v>2887.39</v>
       </c>
       <c r="H5" s="9">
         <f>'Data Sheet'!H43</f>
-        <v>2820.17</v>
       </c>
       <c r="I5" s="9">
         <f>'Data Sheet'!I43</f>
-        <v>2831.75</v>
       </c>
       <c r="J5" s="9">
         <f>'Data Sheet'!J43</f>
-        <v>3161.49</v>
       </c>
       <c r="K5" s="9">
         <f>'Data Sheet'!K43</f>
-        <v>3482.48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
         <f>'Data Sheet'!B50</f>
-        <v>2696.5</v>
       </c>
       <c r="C6" s="1">
         <f>'Data Sheet'!C50</f>
-        <v>3270.68</v>
       </c>
       <c r="D6" s="1">
         <f>'Data Sheet'!D50</f>
-        <v>3689.33</v>
       </c>
       <c r="E6" s="1">
         <f>'Data Sheet'!E50</f>
-        <v>3663.98</v>
       </c>
       <c r="F6" s="1">
         <f>'Data Sheet'!F50</f>
-        <v>4195.68</v>
       </c>
       <c r="G6" s="1">
         <f>'Data Sheet'!G50</f>
-        <v>4009.11</v>
       </c>
       <c r="H6" s="1">
         <f>'Data Sheet'!H50</f>
-        <v>4739.42</v>
       </c>
       <c r="I6" s="1">
         <f>'Data Sheet'!I50</f>
-        <v>4235.2700000000004</v>
       </c>
       <c r="J6" s="1">
         <f>'Data Sheet'!J50</f>
-        <v>4802.0600000000004</v>
       </c>
       <c r="K6" s="1">
         <f>'Data Sheet'!K50</f>
-        <v>5005.96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="9">
         <f>'Data Sheet'!B44</f>
-        <v>284.91000000000003</v>
       </c>
       <c r="C7" s="9">
         <f>'Data Sheet'!C44</f>
-        <v>-884.53</v>
       </c>
       <c r="D7" s="9">
         <f>'Data Sheet'!D44</f>
-        <v>383.68</v>
       </c>
       <c r="E7" s="9">
         <f>'Data Sheet'!E44</f>
-        <v>351.27</v>
       </c>
       <c r="F7" s="9">
         <f>'Data Sheet'!F44</f>
-        <v>506.85</v>
       </c>
       <c r="G7" s="9">
         <f>'Data Sheet'!G44</f>
-        <v>-70.260000000000005</v>
       </c>
       <c r="H7" s="9">
         <f>'Data Sheet'!H44</f>
-        <v>349.16</v>
       </c>
       <c r="I7" s="9">
         <f>'Data Sheet'!I44</f>
-        <v>253.58</v>
       </c>
       <c r="J7" s="9">
         <f>'Data Sheet'!J44</f>
-        <v>246.85</v>
       </c>
       <c r="K7" s="9">
         <f>'Data Sheet'!K44</f>
-        <v>425.62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="9">
         <f>'Data Sheet'!B45</f>
-        <v>883.63</v>
       </c>
       <c r="C8" s="9">
         <f>'Data Sheet'!C45</f>
-        <v>846.36</v>
       </c>
       <c r="D8" s="9">
         <f>'Data Sheet'!D45</f>
-        <v>949.58</v>
       </c>
       <c r="E8" s="9">
         <f>'Data Sheet'!E45</f>
-        <v>974.47</v>
       </c>
       <c r="F8" s="9">
         <f>'Data Sheet'!F45</f>
-        <v>985.32</v>
       </c>
       <c r="G8" s="9">
         <f>'Data Sheet'!G45</f>
-        <v>979.09</v>
       </c>
       <c r="H8" s="9">
         <f>'Data Sheet'!H45</f>
-        <v>1011.87</v>
       </c>
       <c r="I8" s="9">
         <f>'Data Sheet'!I45</f>
-        <v>1076.57</v>
       </c>
       <c r="J8" s="9">
         <f>'Data Sheet'!J45</f>
-        <v>1105.76</v>
       </c>
       <c r="K8" s="9">
         <f>'Data Sheet'!K45</f>
-        <v>1184.73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9">
         <f>'Data Sheet'!B46</f>
-        <v>533.88</v>
       </c>
       <c r="C9" s="9">
         <f>'Data Sheet'!C46</f>
-        <v>622.55999999999995</v>
       </c>
       <c r="D9" s="9">
         <f>'Data Sheet'!D46</f>
-        <v>632.69000000000005</v>
       </c>
       <c r="E9" s="9">
         <f>'Data Sheet'!E46</f>
-        <v>520.1</v>
       </c>
       <c r="F9" s="9">
         <f>'Data Sheet'!F46</f>
-        <v>975.88</v>
       </c>
       <c r="G9" s="9">
         <f>'Data Sheet'!G46</f>
-        <v>618.78</v>
       </c>
       <c r="H9" s="9">
         <f>'Data Sheet'!H46</f>
-        <v>484.06</v>
       </c>
       <c r="I9" s="9">
         <f>'Data Sheet'!I46</f>
-        <v>527.11</v>
       </c>
       <c r="J9" s="9">
         <f>'Data Sheet'!J46</f>
-        <v>923.28</v>
       </c>
       <c r="K9" s="9">
         <f>'Data Sheet'!K46</f>
-        <v>714.92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="9">
         <f>'Data Sheet'!B47</f>
-        <v>1563.9</v>
       </c>
       <c r="C10" s="9">
         <f>'Data Sheet'!C47</f>
-        <v>917.23</v>
       </c>
       <c r="D10" s="9">
         <f>'Data Sheet'!D47</f>
-        <v>2490.7399999999998</v>
       </c>
       <c r="E10" s="9">
         <f>'Data Sheet'!E47</f>
-        <v>2520.6799999999998</v>
       </c>
       <c r="F10" s="9">
         <f>'Data Sheet'!F47</f>
-        <v>2741.33</v>
       </c>
       <c r="G10" s="9">
         <f>'Data Sheet'!G47</f>
-        <v>2340.98</v>
       </c>
       <c r="H10" s="9">
         <f>'Data Sheet'!H47</f>
-        <v>3592.65</v>
       </c>
       <c r="I10" s="9">
         <f>'Data Sheet'!I47</f>
-        <v>2885.17</v>
       </c>
       <c r="J10" s="9">
         <f>'Data Sheet'!J47</f>
-        <v>3019.87</v>
       </c>
       <c r="K10" s="9">
         <f>'Data Sheet'!K47</f>
-        <v>3531.93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="9">
         <f>'Data Sheet'!B48</f>
-        <v>227.39</v>
       </c>
       <c r="C11" s="9">
         <f>'Data Sheet'!C48</f>
-        <v>-221.84</v>
       </c>
       <c r="D11" s="9">
         <f>'Data Sheet'!D48</f>
-        <v>371.36</v>
       </c>
       <c r="E11" s="9">
         <f>'Data Sheet'!E48</f>
-        <v>759.05</v>
       </c>
       <c r="F11" s="9">
         <f>'Data Sheet'!F48</f>
-        <v>533.12</v>
       </c>
       <c r="G11" s="9">
         <f>'Data Sheet'!G48</f>
-        <v>326.20999999999998</v>
       </c>
       <c r="H11" s="9">
         <f>'Data Sheet'!H48</f>
-        <v>485.42</v>
       </c>
       <c r="I11" s="9">
         <f>'Data Sheet'!I48</f>
-        <v>472.63</v>
       </c>
       <c r="J11" s="9">
         <f>'Data Sheet'!J48</f>
-        <v>501.48</v>
       </c>
       <c r="K11" s="9">
         <f>'Data Sheet'!K48</f>
-        <v>508.83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1">
         <f>'Data Sheet'!B49</f>
-        <v>1315.54</v>
       </c>
       <c r="C12" s="1">
         <f>'Data Sheet'!C49</f>
-        <v>1157.55</v>
       </c>
       <c r="D12" s="1">
         <f>'Data Sheet'!D49</f>
-        <v>2114.7199999999998</v>
       </c>
       <c r="E12" s="1">
         <f>'Data Sheet'!E49</f>
-        <v>1747.85</v>
       </c>
       <c r="F12" s="1">
         <f>'Data Sheet'!F49</f>
-        <v>2208.41</v>
       </c>
       <c r="G12" s="1">
         <f>'Data Sheet'!G49</f>
-        <v>2039.66</v>
       </c>
       <c r="H12" s="1">
         <f>'Data Sheet'!H49</f>
-        <v>3112.83</v>
       </c>
       <c r="I12" s="1">
         <f>'Data Sheet'!I49</f>
-        <v>2445</v>
       </c>
       <c r="J12" s="1">
         <f>'Data Sheet'!J49</f>
-        <v>2520.2600000000002</v>
       </c>
       <c r="K12" s="1">
         <f>'Data Sheet'!K49</f>
-        <v>3014.22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="14" t="str">
         <f>IF(B4&gt;0,B6/B4,"")</f>
-        <v>0.56339411262032058</v>
-      </c>
-      <c r="C14" s="14">
+      </c>
+      <c r="C14" s="14" t="str">
         <f t="shared" ref="C14:K14" si="0">IF(C4&gt;0,C6/C4,"")</f>
-        <v>0.56421677290252459</v>
-      </c>
-      <c r="D14" s="14">
+      </c>
+      <c r="D14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>0.59052428551992375</v>
-      </c>
-      <c r="E14" s="14">
+      </c>
+      <c r="E14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>0.55127204009382513</v>
-      </c>
-      <c r="F14" s="14">
+      </c>
+      <c r="F14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>0.60630337711882776</v>
-      </c>
-      <c r="G14" s="14">
+      </c>
+      <c r="G14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>0.58132530993982456</v>
-      </c>
-      <c r="H14" s="14">
+      </c>
+      <c r="H14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>0.62694140819806365</v>
-      </c>
-      <c r="I14" s="14">
+      </c>
+      <c r="I14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>0.59930069534259134</v>
-      </c>
-      <c r="J14" s="14">
+      </c>
+      <c r="J14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>0.60300494126363247</v>
-      </c>
-      <c r="K14" s="14">
+      </c>
+      <c r="K14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>0.58973851496859253</v>
-      </c>
-    </row>
-    <row r="22" s="30" customFormat="1" x14ac:dyDescent="0.25"/>
+      </c>
+    </row>
+    <row r="22" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -3316,22 +3003,20 @@
       <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="11" customWidth="1"/>
-    <col min="3" max="11" width="15.42578125" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="22.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="11" customWidth="1"/>
+    <col min="3" max="11" width="15.5" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="str">
         <f>'Profit &amp; Loss'!A1</f>
-        <v>ADANI PORTS &amp; SPECIAL ECONOMIC ZONE LTD</v>
       </c>
       <c r="E1" t="str">
         <f>UPDATE</f>
-        <v/>
       </c>
       <c r="G1"/>
       <c r="J1" s="4" t="s">
@@ -3339,281 +3024,221 @@
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16">
         <f>'Data Sheet'!B56</f>
-        <v>42460</v>
       </c>
       <c r="C3" s="16">
         <f>'Data Sheet'!C56</f>
-        <v>42825</v>
       </c>
       <c r="D3" s="16">
         <f>'Data Sheet'!D56</f>
-        <v>43190</v>
       </c>
       <c r="E3" s="16">
         <f>'Data Sheet'!E56</f>
-        <v>43555</v>
       </c>
       <c r="F3" s="16">
         <f>'Data Sheet'!F56</f>
-        <v>43921</v>
       </c>
       <c r="G3" s="16">
         <f>'Data Sheet'!G56</f>
-        <v>44286</v>
       </c>
       <c r="H3" s="16">
         <f>'Data Sheet'!H56</f>
-        <v>44651</v>
       </c>
       <c r="I3" s="16">
         <f>'Data Sheet'!I56</f>
-        <v>45016</v>
       </c>
       <c r="J3" s="16">
         <f>'Data Sheet'!J56</f>
-        <v>45382</v>
       </c>
       <c r="K3" s="16">
         <f>'Data Sheet'!K56</f>
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="19">
         <f>'Data Sheet'!B57</f>
-        <v>414.19</v>
       </c>
       <c r="C4" s="19">
         <f>'Data Sheet'!C57</f>
-        <v>414.19</v>
       </c>
       <c r="D4" s="19">
         <f>'Data Sheet'!D57</f>
-        <v>414.19</v>
       </c>
       <c r="E4" s="19">
         <f>'Data Sheet'!E57</f>
-        <v>414.19</v>
       </c>
       <c r="F4" s="19">
         <f>'Data Sheet'!F57</f>
-        <v>406.35</v>
       </c>
       <c r="G4" s="19">
         <f>'Data Sheet'!G57</f>
-        <v>406.35</v>
       </c>
       <c r="H4" s="19">
         <f>'Data Sheet'!H57</f>
-        <v>422.47</v>
       </c>
       <c r="I4" s="19">
         <f>'Data Sheet'!I57</f>
-        <v>432.03</v>
       </c>
       <c r="J4" s="19">
         <f>'Data Sheet'!J57</f>
-        <v>432.03</v>
       </c>
       <c r="K4" s="19">
         <f>'Data Sheet'!K57</f>
-        <v>432.03</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="19">
         <f>'Data Sheet'!B58</f>
-        <v>13091.3</v>
       </c>
       <c r="C5" s="19">
         <f>'Data Sheet'!C58</f>
-        <v>17111.79</v>
       </c>
       <c r="D5" s="19">
         <f>'Data Sheet'!D58</f>
-        <v>20488.759999999998</v>
       </c>
       <c r="E5" s="19">
         <f>'Data Sheet'!E58</f>
-        <v>23958.13</v>
       </c>
       <c r="F5" s="19">
         <f>'Data Sheet'!F58</f>
-        <v>25050.61</v>
       </c>
       <c r="G5" s="19">
         <f>'Data Sheet'!G58</f>
-        <v>30035.38</v>
       </c>
       <c r="H5" s="19">
         <f>'Data Sheet'!H58</f>
-        <v>41399.22</v>
       </c>
       <c r="I5" s="19">
         <f>'Data Sheet'!I58</f>
-        <v>44957.36</v>
       </c>
       <c r="J5" s="19">
         <f>'Data Sheet'!J58</f>
-        <v>52346.21</v>
       </c>
       <c r="K5" s="19">
         <f>'Data Sheet'!K58</f>
-        <v>61836.83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B6" s="19">
         <f>'Data Sheet'!B59</f>
-        <v>22341.53</v>
       </c>
       <c r="C6" s="19">
         <f>'Data Sheet'!C59</f>
-        <v>22214.26</v>
       </c>
       <c r="D6" s="19">
         <f>'Data Sheet'!D59</f>
-        <v>22370.04</v>
       </c>
       <c r="E6" s="19">
         <f>'Data Sheet'!E59</f>
-        <v>27711.54</v>
       </c>
       <c r="F6" s="19">
         <f>'Data Sheet'!F59</f>
-        <v>30242.32</v>
       </c>
       <c r="G6" s="19">
         <f>'Data Sheet'!G59</f>
-        <v>35855.33</v>
       </c>
       <c r="H6" s="19">
         <f>'Data Sheet'!H59</f>
-        <v>47934.75</v>
       </c>
       <c r="I6" s="19">
         <f>'Data Sheet'!I59</f>
-        <v>53434.22</v>
       </c>
       <c r="J6" s="19">
         <f>'Data Sheet'!J59</f>
-        <v>49470.239999999998</v>
       </c>
       <c r="K6" s="19">
         <f>'Data Sheet'!K59</f>
-        <v>51620.73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
       <c r="B7" s="19">
         <f>'Data Sheet'!B60</f>
-        <v>2537.83</v>
       </c>
       <c r="C7" s="19">
         <f>'Data Sheet'!C60</f>
-        <v>3629.13</v>
       </c>
       <c r="D7" s="19">
         <f>'Data Sheet'!D60</f>
-        <v>3959.73</v>
       </c>
       <c r="E7" s="19">
         <f>'Data Sheet'!E60</f>
-        <v>4227.57</v>
       </c>
       <c r="F7" s="19">
         <f>'Data Sheet'!F60</f>
-        <v>6217.42</v>
       </c>
       <c r="G7" s="19">
         <f>'Data Sheet'!G60</f>
-        <v>8284.8700000000008</v>
       </c>
       <c r="H7" s="19">
         <f>'Data Sheet'!H60</f>
-        <v>8571.5499999999993</v>
       </c>
       <c r="I7" s="19">
         <f>'Data Sheet'!I60</f>
-        <v>13739.58</v>
       </c>
       <c r="J7" s="19">
         <f>'Data Sheet'!J60</f>
-        <v>14750.72</v>
       </c>
       <c r="K7" s="19">
         <f>'Data Sheet'!K60</f>
-        <v>19553.060000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="20">
         <f>'Data Sheet'!B61</f>
-        <v>38384.85</v>
       </c>
       <c r="C8" s="20">
         <f>'Data Sheet'!C61</f>
-        <v>43369.37</v>
       </c>
       <c r="D8" s="20">
         <f>'Data Sheet'!D61</f>
-        <v>47232.72</v>
       </c>
       <c r="E8" s="20">
         <f>'Data Sheet'!E61</f>
-        <v>56311.43</v>
       </c>
       <c r="F8" s="20">
         <f>'Data Sheet'!F61</f>
-        <v>61916.7</v>
       </c>
       <c r="G8" s="20">
         <f>'Data Sheet'!G61</f>
-        <v>74581.929999999993</v>
       </c>
       <c r="H8" s="20">
         <f>'Data Sheet'!H61</f>
-        <v>98327.99</v>
       </c>
       <c r="I8" s="20">
         <f>'Data Sheet'!I61</f>
-        <v>112563.19</v>
       </c>
       <c r="J8" s="20">
         <f>'Data Sheet'!J61</f>
-        <v>116999.2</v>
       </c>
       <c r="K8" s="20">
         <f>'Data Sheet'!K61</f>
-        <v>133442.65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -3625,232 +3250,182 @@
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="19">
         <f>'Data Sheet'!B62</f>
-        <v>20883.22</v>
       </c>
       <c r="C10" s="19">
         <f>'Data Sheet'!C62</f>
-        <v>21053.5</v>
       </c>
       <c r="D10" s="19">
         <f>'Data Sheet'!D62</f>
-        <v>22670.01</v>
       </c>
       <c r="E10" s="19">
         <f>'Data Sheet'!E62</f>
-        <v>28121.42</v>
       </c>
       <c r="F10" s="19">
         <f>'Data Sheet'!F62</f>
-        <v>32714.51</v>
       </c>
       <c r="G10" s="19">
         <f>'Data Sheet'!G62</f>
-        <v>48290.96</v>
       </c>
       <c r="H10" s="19">
         <f>'Data Sheet'!H62</f>
-        <v>62552.92</v>
       </c>
       <c r="I10" s="19">
         <f>'Data Sheet'!I62</f>
-        <v>72223.73</v>
       </c>
       <c r="J10" s="19">
         <f>'Data Sheet'!J62</f>
-        <v>75147.81</v>
       </c>
       <c r="K10" s="19">
         <f>'Data Sheet'!K62</f>
-        <v>89616.320000000007</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="19">
         <f>'Data Sheet'!B63</f>
-        <v>1966.76</v>
       </c>
       <c r="C11" s="19">
         <f>'Data Sheet'!C63</f>
-        <v>4513.97</v>
       </c>
       <c r="D11" s="19">
         <f>'Data Sheet'!D63</f>
-        <v>4545.46</v>
       </c>
       <c r="E11" s="19">
         <f>'Data Sheet'!E63</f>
-        <v>4483.4799999999996</v>
       </c>
       <c r="F11" s="19">
         <f>'Data Sheet'!F63</f>
-        <v>3216.33</v>
       </c>
       <c r="G11" s="19">
         <f>'Data Sheet'!G63</f>
-        <v>3697.13</v>
       </c>
       <c r="H11" s="19">
         <f>'Data Sheet'!H63</f>
-        <v>4022.9</v>
       </c>
       <c r="I11" s="19">
         <f>'Data Sheet'!I63</f>
-        <v>6636.77</v>
       </c>
       <c r="J11" s="19">
         <f>'Data Sheet'!J63</f>
-        <v>10936.09</v>
       </c>
       <c r="K11" s="19">
         <f>'Data Sheet'!K63</f>
-        <v>11706.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="19">
         <f>'Data Sheet'!B64</f>
-        <v>545.17999999999995</v>
       </c>
       <c r="C12" s="19">
         <f>'Data Sheet'!C64</f>
-        <v>1161.3599999999999</v>
       </c>
       <c r="D12" s="19">
         <f>'Data Sheet'!D64</f>
-        <v>1078.92</v>
       </c>
       <c r="E12" s="19">
         <f>'Data Sheet'!E64</f>
-        <v>782.3</v>
       </c>
       <c r="F12" s="19">
         <f>'Data Sheet'!F64</f>
-        <v>1178</v>
       </c>
       <c r="G12" s="19">
         <f>'Data Sheet'!G64</f>
-        <v>2236.15</v>
       </c>
       <c r="H12" s="19">
         <f>'Data Sheet'!H64</f>
-        <v>3160.74</v>
       </c>
       <c r="I12" s="19">
         <f>'Data Sheet'!I64</f>
-        <v>7431.65</v>
       </c>
       <c r="J12" s="19">
         <f>'Data Sheet'!J64</f>
-        <v>4288.66</v>
       </c>
       <c r="K12" s="19">
         <f>'Data Sheet'!K64</f>
-        <v>4659.45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>73</v>
       </c>
       <c r="B13" s="19">
         <f>'Data Sheet'!B65</f>
-        <v>14989.69</v>
       </c>
       <c r="C13" s="19">
         <f>'Data Sheet'!C65</f>
-        <v>16640.54</v>
       </c>
       <c r="D13" s="19">
         <f>'Data Sheet'!D65</f>
-        <v>18938.330000000002</v>
       </c>
       <c r="E13" s="19">
         <f>'Data Sheet'!E65</f>
-        <v>22924.23</v>
       </c>
       <c r="F13" s="19">
         <f>'Data Sheet'!F65</f>
-        <v>24807.86</v>
       </c>
       <c r="G13" s="19">
         <f>'Data Sheet'!G65</f>
-        <v>20357.689999999999</v>
       </c>
       <c r="H13" s="19">
         <f>'Data Sheet'!H65</f>
-        <v>28591.43</v>
       </c>
       <c r="I13" s="19">
         <f>'Data Sheet'!I65</f>
-        <v>26271.040000000001</v>
       </c>
       <c r="J13" s="19">
         <f>'Data Sheet'!J65</f>
-        <v>26626.639999999999</v>
       </c>
       <c r="K13" s="19">
         <f>'Data Sheet'!K65</f>
-        <v>27460.78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="19">
         <f>'Data Sheet'!B66</f>
-        <v>38384.85</v>
       </c>
       <c r="C14" s="19">
         <f>'Data Sheet'!C66</f>
-        <v>43369.37</v>
       </c>
       <c r="D14" s="19">
         <f>'Data Sheet'!D66</f>
-        <v>47232.72</v>
       </c>
       <c r="E14" s="19">
         <f>'Data Sheet'!E66</f>
-        <v>56311.43</v>
       </c>
       <c r="F14" s="19">
         <f>'Data Sheet'!F66</f>
-        <v>61916.7</v>
       </c>
       <c r="G14" s="19">
         <f>'Data Sheet'!G66</f>
-        <v>74581.929999999993</v>
       </c>
       <c r="H14" s="19">
         <f>'Data Sheet'!H66</f>
-        <v>98327.99</v>
       </c>
       <c r="I14" s="19">
         <f>'Data Sheet'!I66</f>
-        <v>112563.19</v>
       </c>
       <c r="J14" s="19">
         <f>'Data Sheet'!J66</f>
-        <v>116999.2</v>
       </c>
       <c r="K14" s="19">
         <f>'Data Sheet'!K66</f>
-        <v>133442.65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -3863,319 +3438,250 @@
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="21">
         <f>B13-B7</f>
-        <v>12451.86</v>
       </c>
       <c r="C16" s="21">
         <f t="shared" ref="C16:K16" si="0">C13-C7</f>
-        <v>13011.41</v>
       </c>
       <c r="D16" s="21">
         <f t="shared" si="0"/>
-        <v>14978.600000000002</v>
       </c>
       <c r="E16" s="21">
         <f t="shared" si="0"/>
-        <v>18696.66</v>
       </c>
       <c r="F16" s="21">
         <f t="shared" si="0"/>
-        <v>18590.440000000002</v>
       </c>
       <c r="G16" s="21">
         <f t="shared" si="0"/>
-        <v>12072.819999999998</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" si="0"/>
-        <v>20019.88</v>
       </c>
       <c r="I16" s="21">
         <f t="shared" si="0"/>
-        <v>12531.460000000001</v>
       </c>
       <c r="J16" s="21">
         <f t="shared" si="0"/>
-        <v>11875.92</v>
       </c>
       <c r="K16" s="21">
         <f t="shared" si="0"/>
-        <v>7907.7199999999975</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="21">
         <f>'Data Sheet'!B67</f>
-        <v>2436.09</v>
       </c>
       <c r="C17" s="21">
         <f>'Data Sheet'!C67</f>
-        <v>2692.99</v>
       </c>
       <c r="D17" s="21">
         <f>'Data Sheet'!D67</f>
-        <v>4309.91</v>
       </c>
       <c r="E17" s="21">
         <f>'Data Sheet'!E67</f>
-        <v>2789.66</v>
       </c>
       <c r="F17" s="21">
         <f>'Data Sheet'!F67</f>
-        <v>3202.14</v>
       </c>
       <c r="G17" s="21">
         <f>'Data Sheet'!G67</f>
-        <v>2925.71</v>
       </c>
       <c r="H17" s="21">
         <f>'Data Sheet'!H67</f>
-        <v>2521.14</v>
       </c>
       <c r="I17" s="21">
         <f>'Data Sheet'!I67</f>
-        <v>3957.07</v>
       </c>
       <c r="J17" s="21">
         <f>'Data Sheet'!J67</f>
-        <v>3666.94</v>
       </c>
       <c r="K17" s="21">
         <f>'Data Sheet'!K67</f>
-        <v>4432.3599999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="21">
         <f>'Data Sheet'!B68</f>
-        <v>211.89</v>
       </c>
       <c r="C18" s="21">
         <f>'Data Sheet'!C68</f>
-        <v>657.09</v>
       </c>
       <c r="D18" s="21">
         <f>'Data Sheet'!D68</f>
-        <v>520.29</v>
       </c>
       <c r="E18" s="21">
         <f>'Data Sheet'!E68</f>
-        <v>806.68</v>
       </c>
       <c r="F18" s="21">
         <f>'Data Sheet'!F68</f>
-        <v>288.27999999999997</v>
       </c>
       <c r="G18" s="21">
         <f>'Data Sheet'!G68</f>
-        <v>991.85</v>
       </c>
       <c r="H18" s="21">
         <f>'Data Sheet'!H68</f>
-        <v>395.64</v>
       </c>
       <c r="I18" s="21">
         <f>'Data Sheet'!I68</f>
-        <v>451.97</v>
       </c>
       <c r="J18" s="21">
         <f>'Data Sheet'!J68</f>
-        <v>437.51</v>
       </c>
       <c r="K18" s="21">
         <f>'Data Sheet'!K68</f>
-        <v>521.79999999999995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="5">
         <f>IF('Profit &amp; Loss'!B4&gt;0,'Balance Sheet'!B17/('Profit &amp; Loss'!B4/365),0)</f>
-        <v>125.0832225528054</v>
       </c>
       <c r="C20" s="5">
         <f>IF('Profit &amp; Loss'!C4&gt;0,'Balance Sheet'!C17/('Profit &amp; Loss'!C4/365),0)</f>
-        <v>116.47121520022276</v>
       </c>
       <c r="D20" s="5">
         <f>IF('Profit &amp; Loss'!D4&gt;0,'Balance Sheet'!D17/('Profit &amp; Loss'!D4/365),0)</f>
-        <v>138.93161770420457</v>
       </c>
       <c r="E20" s="5">
         <f>IF('Profit &amp; Loss'!E4&gt;0,'Balance Sheet'!E17/('Profit &amp; Loss'!E4/365),0)</f>
-        <v>93.197701877452985</v>
       </c>
       <c r="F20" s="5">
         <f>IF('Profit &amp; Loss'!F4&gt;0,'Balance Sheet'!F17/('Profit &amp; Loss'!F4/365),0)</f>
-        <v>98.439670615940116</v>
       </c>
       <c r="G20" s="5">
         <f>IF('Profit &amp; Loss'!G4&gt;0,'Balance Sheet'!G17/('Profit &amp; Loss'!G4/365),0)</f>
-        <v>85.093082648052516</v>
       </c>
       <c r="H20" s="5">
         <f>IF('Profit &amp; Loss'!H4&gt;0,'Balance Sheet'!H17/('Profit &amp; Loss'!H4/365),0)</f>
-        <v>53.754739674941973</v>
       </c>
       <c r="I20" s="5">
         <f>IF('Profit &amp; Loss'!I4&gt;0,'Balance Sheet'!I17/('Profit &amp; Loss'!I4/365),0)</f>
-        <v>69.26610320109765</v>
       </c>
       <c r="J20" s="5">
         <f>IF('Profit &amp; Loss'!J4&gt;0,'Balance Sheet'!J17/('Profit &amp; Loss'!J4/365),0)</f>
-        <v>50.108762227373745</v>
       </c>
       <c r="K20" s="5">
         <f>IF('Profit &amp; Loss'!K4&gt;0,'Balance Sheet'!K17/('Profit &amp; Loss'!K4/365),0)</f>
-        <v>53.085935410707606</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="5">
         <f>IF('Balance Sheet'!B18&gt;0,'Profit &amp; Loss'!B4/'Balance Sheet'!B18,0)</f>
-        <v>33.548775307942797</v>
       </c>
       <c r="C21" s="5">
         <f>IF('Balance Sheet'!C18&gt;0,'Profit &amp; Loss'!C4/'Balance Sheet'!C18,0)</f>
-        <v>12.843522196350577</v>
       </c>
       <c r="D21" s="5">
         <f>IF('Balance Sheet'!D18&gt;0,'Profit &amp; Loss'!D4/'Balance Sheet'!D18,0)</f>
-        <v>21.762786138499681</v>
       </c>
       <c r="E21" s="5">
         <f>IF('Balance Sheet'!E18&gt;0,'Profit &amp; Loss'!E4/'Balance Sheet'!E18,0)</f>
-        <v>13.543710021321964</v>
       </c>
       <c r="F21" s="5">
         <f>IF('Balance Sheet'!F18&gt;0,'Profit &amp; Loss'!F4/'Balance Sheet'!F18,0)</f>
-        <v>41.185895657000138</v>
       </c>
       <c r="G21" s="5">
         <f>IF('Balance Sheet'!G18&gt;0,'Profit &amp; Loss'!G4/'Balance Sheet'!G18,0)</f>
-        <v>12.652719665271967</v>
       </c>
       <c r="H21" s="5">
         <f>IF('Balance Sheet'!H18&gt;0,'Profit &amp; Loss'!H4/'Balance Sheet'!H18,0)</f>
-        <v>43.26860277019513</v>
       </c>
       <c r="I21" s="5">
         <f>IF('Balance Sheet'!I18&gt;0,'Profit &amp; Loss'!I4/'Balance Sheet'!I18,0)</f>
-        <v>46.135606345553903</v>
       </c>
       <c r="J21" s="5">
         <f>IF('Balance Sheet'!J18&gt;0,'Profit &amp; Loss'!J4/'Balance Sheet'!J18,0)</f>
-        <v>61.05131311284314</v>
       </c>
       <c r="K21" s="5">
         <f>IF('Balance Sheet'!K18&gt;0,'Profit &amp; Loss'!K4/'Balance Sheet'!K18,0)</f>
-        <v>58.404235339210437</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!B4:B5)&gt;0,'Profit &amp; Loss'!B12/SUM('Balance Sheet'!B4:B5),"")</f>
-        <v>0.21451720744674943</v>
-      </c>
-      <c r="C23" s="14">
+      </c>
+      <c r="C23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!C4:C5)&gt;0,'Profit &amp; Loss'!C12/SUM('Balance Sheet'!C4:C5),"")</f>
-        <v>0.2231840958394338</v>
-      </c>
-      <c r="D23" s="14">
+      </c>
+      <c r="D23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!D4:D5)&gt;0,'Profit &amp; Loss'!D12/SUM('Balance Sheet'!D4:D5),"")</f>
-        <v>0.17574648554390651</v>
-      </c>
-      <c r="E23" s="14">
+      </c>
+      <c r="E23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!E4:E5)&gt;0,'Profit &amp; Loss'!E12/SUM('Balance Sheet'!E4:E5),"")</f>
-        <v>0.1637193340642171</v>
-      </c>
-      <c r="F23" s="14">
+      </c>
+      <c r="F23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!F4:F5)&gt;0,'Profit &amp; Loss'!F12/SUM('Balance Sheet'!F4:F5),"")</f>
-        <v>0.14782322791095245</v>
-      </c>
-      <c r="G23" s="14">
+      </c>
+      <c r="G23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!G4:G5)&gt;0,'Profit &amp; Loss'!G12/SUM('Balance Sheet'!G4:G5),"")</f>
-        <v>0.16406097813757628</v>
-      </c>
-      <c r="H23" s="14">
+      </c>
+      <c r="H23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!H4:H5)&gt;0,'Profit &amp; Loss'!H12/SUM('Balance Sheet'!H4:H5),"")</f>
-        <v>0.11683004680107378</v>
-      </c>
-      <c r="I23" s="14">
+      </c>
+      <c r="I23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!I4:I5)&gt;0,'Profit &amp; Loss'!I12/SUM('Balance Sheet'!I4:I5),"")</f>
-        <v>0.1169623561805964</v>
-      </c>
-      <c r="J23" s="14">
+      </c>
+      <c r="J23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!J4:J5)&gt;0,'Profit &amp; Loss'!J12/SUM('Balance Sheet'!J4:J5),"")</f>
-        <v>0.15367393835035045</v>
-      </c>
-      <c r="K23" s="14">
+      </c>
+      <c r="K23" s="14" t="str">
         <f>IF(SUM('Balance Sheet'!K4:K5)&gt;0,'Profit &amp; Loss'!K12/SUM('Balance Sheet'!K4:K5),"")</f>
-        <v>0.1781357487514626</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B24" s="14"/>
-      <c r="C24" s="14">
+      <c r="C24" s="14" t="str">
         <f>IF((B4+B5+B6+C4+C5+C6)&gt;0,('Profit &amp; Loss'!C10+'Profit &amp; Loss'!C9)*2/(B4+B5+B6+C4+C5+C6),"")</f>
-        <v>0.14009265582586272</v>
-      </c>
-      <c r="D24" s="14">
+      </c>
+      <c r="D24" s="14" t="str">
         <f>IF((C4+C5+C6+D4+D5+D6)&gt;0,('Profit &amp; Loss'!D10+'Profit &amp; Loss'!D9)*2/(C4+C5+C6+D4+D5+D6),"")</f>
-        <v>0.16413745134359906</v>
-      </c>
-      <c r="E24" s="14">
+      </c>
+      <c r="E24" s="14" t="str">
         <f>IF((D4+D5+D6+E4+E5+E6)&gt;0,('Profit &amp; Loss'!E10+'Profit &amp; Loss'!E9)*2/(D4+D5+D6+E4+E5+E6),"")</f>
-        <v>0.1365693183027753</v>
-      </c>
-      <c r="F24" s="14">
+      </c>
+      <c r="F24" s="14" t="str">
         <f>IF((E4+E5+E6+F4+F5+F6)&gt;0,('Profit &amp; Loss'!F10+'Profit &amp; Loss'!F9)*2/(E4+E5+E6+F4+F5+F6),"")</f>
-        <v>0.11494487913415771</v>
-      </c>
-      <c r="G24" s="14">
+      </c>
+      <c r="G24" s="14" t="str">
         <f>IF((F4+F5+F6+G4+G5+G6)&gt;0,('Profit &amp; Loss'!G10+'Profit &amp; Loss'!G9)*2/(F4+F5+F6+G4+G5+G6),"")</f>
-        <v>0.14012387584742295</v>
-      </c>
-      <c r="H24" s="14">
+      </c>
+      <c r="H24" s="14" t="str">
         <f>IF((G4+G5+G6+H4+H5+H6)&gt;0,('Profit &amp; Loss'!H10+'Profit &amp; Loss'!H9)*2/(G4+G5+G6+H4+H5+H6),"")</f>
-        <v>0.10587471604289556</v>
-      </c>
-      <c r="I24" s="14">
+      </c>
+      <c r="I24" s="14" t="str">
         <f>IF((H4+H5+H6+I4+I5+I6)&gt;0,('Profit &amp; Loss'!I10+'Profit &amp; Loss'!I9)*2/(H4+H5+H6+I4+I5+I6),"")</f>
-        <v>8.3248784799876768E-2</v>
-      </c>
-      <c r="J24" s="14">
+      </c>
+      <c r="J24" s="14" t="str">
         <f>IF((I4+I5+I6+J4+J5+J6)&gt;0,('Profit &amp; Loss'!J10+'Profit &amp; Loss'!J9)*2/(I4+I5+I6+J4+J5+J6),"")</f>
-        <v>0.12305546732020342</v>
-      </c>
-      <c r="K24" s="14">
+      </c>
+      <c r="K24" s="14" t="str">
         <f>IF((J4+J5+J6+K4+K5+K6)&gt;0,('Profit &amp; Loss'!K10+'Profit &amp; Loss'!K9)*2/(J4+J5+J6+K4+K5+K6),"")</f>
-        <v>0.14399536370432103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -4200,22 +3706,20 @@
       <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="13.42578125" style="6" customWidth="1"/>
-    <col min="7" max="11" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="26.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="13.5" style="6" customWidth="1"/>
+    <col min="7" max="11" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="str">
         <f>'Balance Sheet'!A1</f>
-        <v>ADANI PORTS &amp; SPECIAL ECONOMIC ZONE LTD</v>
       </c>
       <c r="E1" t="str">
         <f>UPDATE</f>
-        <v/>
       </c>
       <c r="F1"/>
       <c r="J1" s="4" t="s">
@@ -4223,232 +3727,182 @@
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="16">
         <f>'Data Sheet'!B81</f>
-        <v>42460</v>
       </c>
       <c r="C3" s="16">
         <f>'Data Sheet'!C81</f>
-        <v>42825</v>
       </c>
       <c r="D3" s="16">
         <f>'Data Sheet'!D81</f>
-        <v>43190</v>
       </c>
       <c r="E3" s="16">
         <f>'Data Sheet'!E81</f>
-        <v>43555</v>
       </c>
       <c r="F3" s="16">
         <f>'Data Sheet'!F81</f>
-        <v>43921</v>
       </c>
       <c r="G3" s="16">
         <f>'Data Sheet'!G81</f>
-        <v>44286</v>
       </c>
       <c r="H3" s="16">
         <f>'Data Sheet'!H81</f>
-        <v>44651</v>
       </c>
       <c r="I3" s="16">
         <f>'Data Sheet'!I81</f>
-        <v>45016</v>
       </c>
       <c r="J3" s="16">
         <f>'Data Sheet'!J81</f>
-        <v>45382</v>
       </c>
       <c r="K3" s="16">
         <f>'Data Sheet'!K81</f>
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="1">
         <f>'Data Sheet'!B82</f>
-        <v>2380.52</v>
       </c>
       <c r="C4" s="1">
         <f>'Data Sheet'!C82</f>
-        <v>4062.57</v>
       </c>
       <c r="D4" s="1">
         <f>'Data Sheet'!D82</f>
-        <v>5608.14</v>
       </c>
       <c r="E4" s="1">
         <f>'Data Sheet'!E82</f>
-        <v>6029.4</v>
       </c>
       <c r="F4" s="1">
         <f>'Data Sheet'!F82</f>
-        <v>7401.81</v>
       </c>
       <c r="G4" s="1">
         <f>'Data Sheet'!G82</f>
-        <v>7555.78</v>
       </c>
       <c r="H4" s="1">
         <f>'Data Sheet'!H82</f>
-        <v>10420.14</v>
       </c>
       <c r="I4" s="1">
         <f>'Data Sheet'!I82</f>
-        <v>11899.5</v>
       </c>
       <c r="J4" s="1">
         <f>'Data Sheet'!J82</f>
-        <v>15017.58</v>
       </c>
       <c r="K4" s="1">
         <f>'Data Sheet'!K82</f>
-        <v>17226.28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9">
         <f>'Data Sheet'!B83</f>
-        <v>-4153.16</v>
       </c>
       <c r="C5" s="9">
         <f>'Data Sheet'!C83</f>
-        <v>-2629.15</v>
       </c>
       <c r="D5" s="9">
         <f>'Data Sheet'!D83</f>
-        <v>-3845.84</v>
       </c>
       <c r="E5" s="9">
         <f>'Data Sheet'!E83</f>
-        <v>-4368.03</v>
       </c>
       <c r="F5" s="9">
         <f>'Data Sheet'!F83</f>
-        <v>-748.91</v>
       </c>
       <c r="G5" s="9">
         <f>'Data Sheet'!G83</f>
-        <v>-14064.12</v>
       </c>
       <c r="H5" s="9">
         <f>'Data Sheet'!H83</f>
-        <v>-5493.13</v>
       </c>
       <c r="I5" s="9">
         <f>'Data Sheet'!I83</f>
-        <v>-16715.93</v>
       </c>
       <c r="J5" s="9">
         <f>'Data Sheet'!J83</f>
-        <v>-6946.55</v>
       </c>
       <c r="K5" s="9">
         <f>'Data Sheet'!K83</f>
-        <v>-9787.5300000000007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="9">
         <f>'Data Sheet'!B84</f>
-        <v>2170.41</v>
       </c>
       <c r="C6" s="9">
         <f>'Data Sheet'!C84</f>
-        <v>-1324.71</v>
       </c>
       <c r="D6" s="9">
         <f>'Data Sheet'!D84</f>
-        <v>-1889.03</v>
       </c>
       <c r="E6" s="9">
         <f>'Data Sheet'!E84</f>
-        <v>2313.34</v>
       </c>
       <c r="F6" s="9">
         <f>'Data Sheet'!F84</f>
-        <v>-4255.63</v>
       </c>
       <c r="G6" s="9">
         <f>'Data Sheet'!G84</f>
-        <v>3513.85</v>
       </c>
       <c r="H6" s="9">
         <f>'Data Sheet'!H84</f>
-        <v>-585.77</v>
       </c>
       <c r="I6" s="9">
         <f>'Data Sheet'!I84</f>
-        <v>-2733.8</v>
       </c>
       <c r="J6" s="9">
         <f>'Data Sheet'!J84</f>
-        <v>-7800.11</v>
       </c>
       <c r="K6" s="9">
         <f>'Data Sheet'!K84</f>
-        <v>-6915.52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="1">
         <f>'Data Sheet'!B85</f>
-        <v>397.77</v>
       </c>
       <c r="C7" s="1">
         <f>'Data Sheet'!C85</f>
-        <v>108.71</v>
       </c>
       <c r="D7" s="1">
         <f>'Data Sheet'!D85</f>
-        <v>-126.73</v>
       </c>
       <c r="E7" s="1">
         <f>'Data Sheet'!E85</f>
-        <v>3974.71</v>
       </c>
       <c r="F7" s="1">
         <f>'Data Sheet'!F85</f>
-        <v>2397.27</v>
       </c>
       <c r="G7" s="1">
         <f>'Data Sheet'!G85</f>
-        <v>-2994.49</v>
       </c>
       <c r="H7" s="1">
         <f>'Data Sheet'!H85</f>
-        <v>4341.24</v>
       </c>
       <c r="I7" s="1">
         <f>'Data Sheet'!I85</f>
-        <v>-7550.23</v>
       </c>
       <c r="J7" s="1">
         <f>'Data Sheet'!J85</f>
-        <v>270.92</v>
       </c>
       <c r="K7" s="1">
         <f>'Data Sheet'!K85</f>
-        <v>523.23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -4461,7 +3915,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="24" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -4481,42 +3935,42 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="8"/>
-    <col min="2" max="2" width="10.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="26" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="11"/>
-    <col min="6" max="6" width="6.85546875" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="8.83203125" style="8"/>
+    <col min="2" max="2" width="10.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="26" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="11"/>
+    <col min="6" max="6" width="6.83203125" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>51</v>
       </c>
@@ -4524,27 +3978,27 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>92</v>
       </c>
@@ -4570,14 +4024,14 @@
       <selection pane="bottomRight" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="27.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4586,7 +4040,6 @@
       </c>
       <c r="E1" s="32" t="str">
         <f>IF(B2&lt;&gt;B3, "A NEW VERSION OF THE WORKSHEET IS AVAILABLE", "")</f>
-        <v/>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -4595,7 +4048,7 @@
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -4612,7 +4065,7 @@
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -4620,88 +4073,87 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="5">
         <f>IF(B9&gt;0, B9/B8, 0)</f>
-        <v>216.01392023237628</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.00</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B8">
-        <v>1342.65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1349.30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B9">
-        <v>290031.09000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>291467.55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="16">
-        <v>42460</v>
+        <v>42460.0</v>
       </c>
       <c r="C16" s="16">
-        <v>42825</v>
+        <v>42825.0</v>
       </c>
       <c r="D16" s="16">
-        <v>43190</v>
+        <v>43190.0</v>
       </c>
       <c r="E16" s="16">
-        <v>43555</v>
+        <v>43555.0</v>
       </c>
       <c r="F16" s="16">
-        <v>43921</v>
+        <v>43921.0</v>
       </c>
       <c r="G16" s="16">
-        <v>44286</v>
+        <v>44286.0</v>
       </c>
       <c r="H16" s="16">
-        <v>44651</v>
+        <v>44651.0</v>
       </c>
       <c r="I16" s="16">
-        <v>45016</v>
+        <v>45016.0</v>
       </c>
       <c r="J16" s="16">
-        <v>45382</v>
+        <v>45382.0</v>
       </c>
       <c r="K16" s="16">
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>45747.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
@@ -4730,13 +4182,13 @@
         <v>20851.91</v>
       </c>
       <c r="J17">
-        <v>26710.560000000001</v>
+        <v>26710.56</v>
       </c>
       <c r="K17">
         <v>30475.33</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -4750,12 +4202,12 @@
         <v>140.43</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -4787,10 +4239,10 @@
         <v>1228.57</v>
       </c>
       <c r="K20">
-        <v>1267.3499999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1267.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -4816,7 +4268,7 @@
         <v>3950.79</v>
       </c>
       <c r="I21">
-        <v>4742.2700000000004</v>
+        <v>4742.27</v>
       </c>
       <c r="J21">
         <v>6048.03</v>
@@ -4825,7 +4277,7 @@
         <v>7003.68</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -4839,7 +4291,7 @@
         <v>448.15</v>
       </c>
       <c r="E22">
-        <v>530.54999999999995</v>
+        <v>530.55</v>
       </c>
       <c r="F22">
         <v>547.66</v>
@@ -4860,7 +4312,7 @@
         <v>2011.44</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>85</v>
       </c>
@@ -4895,7 +4347,7 @@
         <v>1424.27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>86</v>
       </c>
@@ -4909,7 +4361,7 @@
         <v>111.88</v>
       </c>
       <c r="E24">
-        <v>591.42999999999995</v>
+        <v>591.43</v>
       </c>
       <c r="F24">
         <v>1796.26</v>
@@ -4918,7 +4370,7 @@
         <v>-558.22</v>
       </c>
       <c r="H24">
-        <v>1057.3399999999999</v>
+        <v>1057.34</v>
       </c>
       <c r="I24">
         <v>2135.9</v>
@@ -4927,10 +4379,10 @@
         <v>525.13</v>
       </c>
       <c r="K24">
-        <v>628.07000000000005</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>628.07</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>9</v>
       </c>
@@ -4965,7 +4417,7 @@
         <v>1799.85</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>10</v>
       </c>
@@ -4976,7 +4428,7 @@
         <v>1160.19</v>
       </c>
       <c r="D26">
-        <v>1188.3699999999999</v>
+        <v>1188.37</v>
       </c>
       <c r="E26">
         <v>1373.48</v>
@@ -5000,7 +4452,7 @@
         <v>4378.93</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
@@ -5032,10 +4484,10 @@
         <v>2732.94</v>
       </c>
       <c r="K27">
-        <v>2531.8200000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2531.82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>12</v>
       </c>
@@ -5070,7 +4522,7 @@
         <v>13029.62</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>13</v>
       </c>
@@ -5105,7 +4557,7 @@
         <v>1968.36</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>14</v>
       </c>
@@ -5140,7 +4592,7 @@
         <v>11092.31</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>70</v>
       </c>
@@ -5148,7 +4600,7 @@
         <v>227.8</v>
       </c>
       <c r="C31">
-        <v>269.22000000000003</v>
+        <v>269.22</v>
       </c>
       <c r="D31">
         <v>414.19</v>
@@ -5169,75 +4621,75 @@
         <v>1080.08</v>
       </c>
       <c r="J31">
-        <v>1296.0899999999999</v>
+        <v>1296.09</v>
       </c>
       <c r="K31">
         <v>1512.1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="16">
-        <v>44926</v>
+        <v>44926.0</v>
       </c>
       <c r="C41" s="16">
-        <v>45016</v>
+        <v>45016.0</v>
       </c>
       <c r="D41" s="16">
-        <v>45107</v>
+        <v>45107.0</v>
       </c>
       <c r="E41" s="16">
-        <v>45199</v>
+        <v>45199.0</v>
       </c>
       <c r="F41" s="16">
-        <v>45291</v>
+        <v>45291.0</v>
       </c>
       <c r="G41" s="16">
-        <v>45382</v>
+        <v>45382.0</v>
       </c>
       <c r="H41" s="16">
-        <v>45473</v>
+        <v>45473.0</v>
       </c>
       <c r="I41" s="16">
-        <v>45565</v>
+        <v>45565.0</v>
       </c>
       <c r="J41" s="16">
-        <v>45657</v>
+        <v>45657.0</v>
       </c>
       <c r="K41" s="16">
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>45747.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>6</v>
       </c>
@@ -5272,7 +4724,7 @@
         <v>8488.44</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>7</v>
       </c>
@@ -5283,7 +4735,7 @@
         <v>2526.17</v>
       </c>
       <c r="D43">
-        <v>2558.2199999999998</v>
+        <v>2558.22</v>
       </c>
       <c r="E43">
         <v>2982.43</v>
@@ -5307,12 +4759,12 @@
         <v>3482.48</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B44">
-        <v>284.91000000000003</v>
+        <v>284.91</v>
       </c>
       <c r="C44">
         <v>-884.53</v>
@@ -5327,7 +4779,7 @@
         <v>506.85</v>
       </c>
       <c r="G44">
-        <v>-70.260000000000005</v>
+        <v>-70.26</v>
       </c>
       <c r="H44">
         <v>349.16</v>
@@ -5342,7 +4794,7 @@
         <v>425.62</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>10</v>
       </c>
@@ -5377,7 +4829,7 @@
         <v>1184.73</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>11</v>
       </c>
@@ -5385,10 +4837,10 @@
         <v>533.88</v>
       </c>
       <c r="C46">
-        <v>622.55999999999995</v>
+        <v>622.56</v>
       </c>
       <c r="D46">
-        <v>632.69000000000005</v>
+        <v>632.69</v>
       </c>
       <c r="E46">
         <v>520.1</v>
@@ -5412,7 +4864,7 @@
         <v>714.92</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>12</v>
       </c>
@@ -5423,10 +4875,10 @@
         <v>917.23</v>
       </c>
       <c r="D47">
-        <v>2490.7399999999998</v>
+        <v>2490.74</v>
       </c>
       <c r="E47">
-        <v>2520.6799999999998</v>
+        <v>2520.68</v>
       </c>
       <c r="F47">
         <v>2741.33</v>
@@ -5447,7 +4899,7 @@
         <v>3531.93</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>13</v>
       </c>
@@ -5467,7 +4919,7 @@
         <v>533.12</v>
       </c>
       <c r="G48">
-        <v>326.20999999999998</v>
+        <v>326.21</v>
       </c>
       <c r="H48">
         <v>485.42</v>
@@ -5482,7 +4934,7 @@
         <v>508.83</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>14</v>
       </c>
@@ -5493,7 +4945,7 @@
         <v>1157.55</v>
       </c>
       <c r="D49">
-        <v>2114.7199999999998</v>
+        <v>2114.72</v>
       </c>
       <c r="E49">
         <v>1747.85</v>
@@ -5508,16 +4960,16 @@
         <v>3112.83</v>
       </c>
       <c r="I49">
-        <v>2445</v>
+        <v>2445.0</v>
       </c>
       <c r="J49">
-        <v>2520.2600000000002</v>
+        <v>2520.26</v>
       </c>
       <c r="K49">
         <v>3014.22</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>8</v>
       </c>
@@ -5543,68 +4995,68 @@
         <v>4739.42</v>
       </c>
       <c r="I50">
-        <v>4235.2700000000004</v>
+        <v>4235.27</v>
       </c>
       <c r="J50">
-        <v>4802.0600000000004</v>
+        <v>4802.06</v>
       </c>
       <c r="K50">
         <v>5005.96</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B56" s="16">
-        <v>42460</v>
+        <v>42460.0</v>
       </c>
       <c r="C56" s="16">
-        <v>42825</v>
+        <v>42825.0</v>
       </c>
       <c r="D56" s="16">
-        <v>43190</v>
+        <v>43190.0</v>
       </c>
       <c r="E56" s="16">
-        <v>43555</v>
+        <v>43555.0</v>
       </c>
       <c r="F56" s="16">
-        <v>43921</v>
+        <v>43921.0</v>
       </c>
       <c r="G56" s="16">
-        <v>44286</v>
+        <v>44286.0</v>
       </c>
       <c r="H56" s="16">
-        <v>44651</v>
+        <v>44651.0</v>
       </c>
       <c r="I56" s="16">
-        <v>45016</v>
+        <v>45016.0</v>
       </c>
       <c r="J56" s="16">
-        <v>45382</v>
+        <v>45382.0</v>
       </c>
       <c r="K56" s="16">
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45747.0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>24</v>
       </c>
@@ -5639,7 +5091,7 @@
         <v>432.03</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
         <v>25</v>
       </c>
@@ -5650,7 +5102,7 @@
         <v>17111.79</v>
       </c>
       <c r="D58">
-        <v>20488.759999999998</v>
+        <v>20488.76</v>
       </c>
       <c r="E58">
         <v>23958.13</v>
@@ -5674,7 +5126,7 @@
         <v>61836.83</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>71</v>
       </c>
@@ -5703,13 +5155,13 @@
         <v>53434.22</v>
       </c>
       <c r="J59">
-        <v>49470.239999999998</v>
+        <v>49470.24</v>
       </c>
       <c r="K59">
         <v>51620.73</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>72</v>
       </c>
@@ -5729,10 +5181,10 @@
         <v>6217.42</v>
       </c>
       <c r="G60">
-        <v>8284.8700000000008</v>
+        <v>8284.87</v>
       </c>
       <c r="H60">
-        <v>8571.5499999999993</v>
+        <v>8571.55</v>
       </c>
       <c r="I60">
         <v>13739.58</v>
@@ -5741,10 +5193,10 @@
         <v>14750.72</v>
       </c>
       <c r="K60">
-        <v>19553.060000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>19553.06</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>26</v>
       </c>
@@ -5764,7 +5216,7 @@
         <v>61916.7</v>
       </c>
       <c r="G61">
-        <v>74581.929999999993</v>
+        <v>74581.93</v>
       </c>
       <c r="H61">
         <v>98327.99</v>
@@ -5779,7 +5231,7 @@
         <v>133442.65</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>27</v>
       </c>
@@ -5811,10 +5263,10 @@
         <v>75147.81</v>
       </c>
       <c r="K62">
-        <v>89616.320000000007</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+        <v>89616.32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>28</v>
       </c>
@@ -5828,7 +5280,7 @@
         <v>4545.46</v>
       </c>
       <c r="E63">
-        <v>4483.4799999999996</v>
+        <v>4483.48</v>
       </c>
       <c r="F63">
         <v>3216.33</v>
@@ -5849,15 +5301,15 @@
         <v>11706.1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B64">
-        <v>545.17999999999995</v>
+        <v>545.18</v>
       </c>
       <c r="C64">
-        <v>1161.3599999999999</v>
+        <v>1161.36</v>
       </c>
       <c r="D64">
         <v>1078.92</v>
@@ -5866,7 +5318,7 @@
         <v>782.3</v>
       </c>
       <c r="F64">
-        <v>1178</v>
+        <v>1178.0</v>
       </c>
       <c r="G64">
         <v>2236.15</v>
@@ -5884,7 +5336,7 @@
         <v>4659.45</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>73</v>
       </c>
@@ -5895,7 +5347,7 @@
         <v>16640.54</v>
       </c>
       <c r="D65">
-        <v>18938.330000000002</v>
+        <v>18938.33</v>
       </c>
       <c r="E65">
         <v>22924.23</v>
@@ -5904,22 +5356,22 @@
         <v>24807.86</v>
       </c>
       <c r="G65">
-        <v>20357.689999999999</v>
+        <v>20357.69</v>
       </c>
       <c r="H65">
         <v>28591.43</v>
       </c>
       <c r="I65">
-        <v>26271.040000000001</v>
+        <v>26271.04</v>
       </c>
       <c r="J65">
-        <v>26626.639999999999</v>
+        <v>26626.64</v>
       </c>
       <c r="K65">
         <v>27460.78</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>26</v>
       </c>
@@ -5939,7 +5391,7 @@
         <v>61916.7</v>
       </c>
       <c r="G66">
-        <v>74581.929999999993</v>
+        <v>74581.93</v>
       </c>
       <c r="H66">
         <v>98327.99</v>
@@ -5954,7 +5406,7 @@
         <v>133442.65</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>78</v>
       </c>
@@ -5986,10 +5438,10 @@
         <v>3666.94</v>
       </c>
       <c r="K67">
-        <v>4432.3599999999997</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4432.36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>45</v>
       </c>
@@ -6006,7 +5458,7 @@
         <v>806.68</v>
       </c>
       <c r="F68">
-        <v>288.27999999999997</v>
+        <v>288.28</v>
       </c>
       <c r="G68">
         <v>991.85</v>
@@ -6021,10 +5473,10 @@
         <v>437.51</v>
       </c>
       <c r="K68">
-        <v>521.79999999999995</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+        <v>521.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>87</v>
       </c>
@@ -6050,7 +5502,7 @@
         <v>10667.41</v>
       </c>
       <c r="I69">
-        <v>4334.3100000000004</v>
+        <v>4334.31</v>
       </c>
       <c r="J69">
         <v>7631.88</v>
@@ -6059,140 +5511,140 @@
         <v>6605.97</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B70">
-        <v>2070951761</v>
+        <v>2070951761.0</v>
       </c>
       <c r="C70">
-        <v>2070951761</v>
+        <v>2070951761.0</v>
       </c>
       <c r="D70">
-        <v>2070951761</v>
+        <v>2070951761.0</v>
       </c>
       <c r="E70">
-        <v>2070951761</v>
+        <v>2070951761.0</v>
       </c>
       <c r="F70">
-        <v>2031751761</v>
+        <v>2031751761.0</v>
       </c>
       <c r="G70">
-        <v>2031751761</v>
+        <v>2031751761.0</v>
       </c>
       <c r="H70">
-        <v>2112373230</v>
+        <v>2112373230.0</v>
       </c>
       <c r="I70">
-        <v>2160138945</v>
+        <v>2160138945.0</v>
       </c>
       <c r="J70">
-        <v>2160138945</v>
+        <v>2160138945.0</v>
       </c>
       <c r="K70">
-        <v>2160138945</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2160138945.0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="E72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="F72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="G72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="H72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="J72">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="K72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="9"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="9"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="9"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="9"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="9"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="9"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B81" s="16">
-        <v>42460</v>
+        <v>42460.0</v>
       </c>
       <c r="C81" s="16">
-        <v>42825</v>
+        <v>42825.0</v>
       </c>
       <c r="D81" s="16">
-        <v>43190</v>
+        <v>43190.0</v>
       </c>
       <c r="E81" s="16">
-        <v>43555</v>
+        <v>43555.0</v>
       </c>
       <c r="F81" s="16">
-        <v>43921</v>
+        <v>43921.0</v>
       </c>
       <c r="G81" s="16">
-        <v>44286</v>
+        <v>44286.0</v>
       </c>
       <c r="H81" s="16">
-        <v>44651</v>
+        <v>44651.0</v>
       </c>
       <c r="I81" s="16">
-        <v>45016</v>
+        <v>45016.0</v>
       </c>
       <c r="J81" s="16">
-        <v>45382</v>
+        <v>45382.0</v>
       </c>
       <c r="K81" s="16">
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>45747.0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
         <v>32</v>
       </c>
@@ -6227,7 +5679,7 @@
         <v>17226.28</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
         <v>33</v>
       </c>
@@ -6259,10 +5711,10 @@
         <v>-6946.55</v>
       </c>
       <c r="K83">
-        <v>-9787.5300000000007</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>-9787.53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
         <v>34</v>
       </c>
@@ -6297,7 +5749,7 @@
         <v>-6915.52</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>35</v>
       </c>
@@ -6332,19 +5784,19 @@
         <v>523.23</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="9"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="9"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="9"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="9"/>
     </row>
-    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>77</v>
       </c>
@@ -6379,12 +5831,12 @@
         <v>1182.95</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>89</v>
       </c>

</xml_diff>